<commit_message>
text_summ: added resume training from checkpoint
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B720ABBA-1E0E-4186-99BC-FBA3F3F3F383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF8CA6E-E6C8-436E-B946-BBCA667E4559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="logs-1" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="111">
   <si>
     <t>Log ID</t>
   </si>
@@ -374,6 +374,9 @@
   </si>
   <si>
     <t>Okay</t>
+  </si>
+  <si>
+    <t>Good</t>
   </si>
 </sst>
 </file>
@@ -3883,11 +3886,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P20" sqref="P20"/>
+      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5029,6 +5032,70 @@
       <c r="R19">
         <v>1.37</v>
       </c>
+      <c r="S19" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>89</v>
+      </c>
+      <c r="B20" s="2" t="str">
+        <f>CONCATENATE(D20,"_lora-",F20,"_ebs-",H20*J20,"_lr-",K20,"-",L20,"_pt2")</f>
+        <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2</v>
+      </c>
+      <c r="C20" s="2" t="str">
+        <f>CONCATENATE(D20,"_uf-",E20,"_lora-",F20,"_nepoch-",G20,"_ebs-",H20*J20,"_lr-",K20,"-",L20,"_drop-",M20,"_wd-",N20)</f>
+        <v>bart-base_uf-none_lora-512-512-0_nepoch-30_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G20">
+        <v>30</v>
+      </c>
+      <c r="H20">
+        <v>2</v>
+      </c>
+      <c r="I20">
+        <v>2</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20" t="s">
+        <v>6</v>
+      </c>
+      <c r="P20">
+        <v>0.3</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>110</v>
+      </c>
+      <c r="R20">
+        <v>1.5</v>
+      </c>
+      <c r="S20" t="s">
+        <v>103</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S1" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}"/>

</xml_diff>

<commit_message>
text_summ: this is the issue observed in both my models and har1 model: training predictions are very good, validation predictions are very poor. Performance is about the same. Next to investigate: dataset problems?
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FF8CA6E-E6C8-436E-B946-BBCA667E4559}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70356F9-C959-42B2-81ED-2CF5E06C5CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'logs-1'!$A$1:$Q$102</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$S$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="619" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="117">
   <si>
     <t>Log ID</t>
   </si>
@@ -377,6 +377,24 @@
   </si>
   <si>
     <t>Good</t>
+  </si>
+  <si>
+    <t>step-1-0.9992</t>
+  </si>
+  <si>
+    <t>step-1-0.9994</t>
+  </si>
+  <si>
+    <t>Dataset</t>
+  </si>
+  <si>
+    <t>ogtvsplit</t>
+  </si>
+  <si>
+    <t>tvtsplit</t>
+  </si>
+  <si>
+    <t>Use original dataset</t>
   </si>
 </sst>
 </file>
@@ -3886,36 +3904,37 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q21" sqref="Q21"/>
+      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="53.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="26" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="26" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>101</v>
       </c>
@@ -3926,174 +3945,183 @@
         <v>83</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="N1" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>87</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f>CONCATENATE(D2,"_uf-",E2,"_ebs-",H2*J2,"_lr-",K2,"-",L2)</f>
+        <f>CONCATENATE(E2,"_uf-",F2,"_ebs-",I2*K2,"_lr-",L2,"-",M2)</f>
         <v>bart-base_uf-all_ebs-8_lr-0.00005-step-1-0.998</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>CONCATENATE(D2,"_uf-",E2,"_lora-",F2,"_nepoch-",G2,"_ebs-",H2*J2,"_lr-",K2,"-",L2,"_drop-",M2,"_wd-",N2)</f>
+        <f>CONCATENATE(E2,"_uf-",F2,"_lora-",G2,"_nepoch-",H2,"_ebs-",I2*K2,"_lr-",L2,"-",M2,"_drop-",N2,"_wd-",O2)</f>
         <v>bart-base_uf-all_lora-none_nepoch-30_ebs-8_lr-0.00005-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
+      <c r="D2" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" t="s">
         <v>79</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>30</v>
       </c>
-      <c r="H2">
-        <v>2</v>
-      </c>
       <c r="I2">
         <v>2</v>
       </c>
       <c r="J2">
-        <v>4</v>
-      </c>
-      <c r="K2" s="1">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>4</v>
+      </c>
+      <c r="L2" s="1">
         <v>5.0000000000000002E-5</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2">
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q2">
         <v>0.6</v>
       </c>
-      <c r="R2">
+      <c r="S2">
         <v>1.2</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>87</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B4" si="0">CONCATENATE(D3,"_uf-",E3,"_ebs-",H3*J3,"_lr-",K3,"-",L3)</f>
+        <f t="shared" ref="B3:B4" si="0">CONCATENATE(E3,"_uf-",F3,"_ebs-",I3*K3,"_lr-",L3,"-",M3)</f>
         <v>bart-base_uf-all_ebs-8_lr-0.0001-step-1-0.998</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>CONCATENATE(D3,"_uf-",E3,"_lora-",F3,"_nepoch-",G3,"_ebs-",H3*J3,"_lr-",K3,"-",L3,"_drop-",M3,"_wd-",N3)</f>
+        <f>CONCATENATE(E3,"_uf-",F3,"_lora-",G3,"_nepoch-",H3,"_ebs-",I3*K3,"_lr-",L3,"-",M3,"_drop-",N3,"_wd-",O3)</f>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0001-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D3" t="s">
-        <v>2</v>
+      <c r="D3" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
         <v>79</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G3">
-        <v>15</v>
-      </c>
       <c r="H3">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I3">
         <v>2</v>
       </c>
       <c r="J3">
-        <v>4</v>
-      </c>
-      <c r="K3" s="1">
+        <v>2</v>
+      </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
+      <c r="L3" s="1">
         <v>1E-4</v>
       </c>
-      <c r="L3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="N3" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P3">
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3">
         <v>0.4</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>95</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>1.3</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>87</v>
       </c>
@@ -4102,1003 +4130,1271 @@
         <v>bart-base_uf-all_ebs-8_lr-0.0002-step-1-0.998</v>
       </c>
       <c r="C4" s="2" t="str">
-        <f>CONCATENATE(D4,"_uf-",E4,"_lora-",F4,"_nepoch-",G4,"_ebs-",H4*J4,"_lr-",K4,"-",L4,"_drop-",M4,"_wd-",N4)</f>
+        <f>CONCATENATE(E4,"_uf-",F4,"_lora-",G4,"_nepoch-",H4,"_ebs-",I4*K4,"_lr-",L4,"-",M4,"_drop-",N4,"_wd-",O4)</f>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0002-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D4" t="s">
-        <v>2</v>
+      <c r="D4" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
         <v>79</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G4">
-        <v>15</v>
-      </c>
       <c r="H4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I4">
         <v>2</v>
       </c>
       <c r="J4">
-        <v>4</v>
-      </c>
-      <c r="K4" s="1">
+        <v>2</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+      <c r="L4" s="1">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="L4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M4" s="2" t="s">
+      <c r="N4" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N4">
-        <v>0</v>
-      </c>
-      <c r="O4" t="s">
-        <v>6</v>
-      </c>
-      <c r="P4">
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q4">
         <v>0.2</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>94</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>1.5</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>87</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f t="shared" ref="B5" si="1">CONCATENATE(D5,"_uf-",E5,"_ebs-",H5*J5,"_lr-",K5,"-",L5)</f>
+        <f t="shared" ref="B5" si="1">CONCATENATE(E5,"_uf-",F5,"_ebs-",I5*K5,"_lr-",L5,"-",M5)</f>
         <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f>CONCATENATE(D5,"_uf-",E5,"_lora-",F5,"_nepoch-",G5,"_ebs-",H5*J5,"_lr-",K5,"-",L5,"_drop-",M5,"_wd-",N5)</f>
+        <f>CONCATENATE(E5,"_uf-",F5,"_lora-",G5,"_nepoch-",H5,"_ebs-",I5*K5,"_lr-",L5,"-",M5,"_drop-",N5,"_wd-",O5)</f>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D5" t="s">
-        <v>2</v>
+      <c r="D5" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="G5" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="G5">
-        <v>15</v>
-      </c>
       <c r="H5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="J5">
-        <v>4</v>
-      </c>
-      <c r="K5" s="1">
+        <v>2</v>
+      </c>
+      <c r="K5">
+        <v>4</v>
+      </c>
+      <c r="L5" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="L5" s="2" t="s">
+      <c r="M5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M5" s="2" t="s">
+      <c r="N5" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5" t="s">
-        <v>6</v>
-      </c>
-      <c r="P5">
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q5">
         <v>0.1</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>94</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>1.8</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>89</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f>CONCATENATE(D6,"_lora-",F6,"_ebs-",H6*J6,"_lr-",K6,"-",L6)</f>
+        <f>CONCATENATE(E6,"_lora-",G6,"_ebs-",I6*K6,"_lr-",L6,"-",M6)</f>
         <v>bart-base_lora-8-32-0_ebs-8_lr-0.0004-step-1-0.998</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f>CONCATENATE(D6,"_uf-",E6,"_lora-",F6,"_nepoch-",G6,"_ebs-",H6*J6,"_lr-",K6,"-",L6,"_drop-",M6,"_wd-",N6)</f>
+        <f>CONCATENATE(E6,"_uf-",F6,"_lora-",G6,"_nepoch-",H6,"_ebs-",I6*K6,"_lr-",L6,"-",M6,"_drop-",N6,"_wd-",O6)</f>
         <v>bart-base_uf-none_lora-8-32-0_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D6" t="s">
-        <v>2</v>
+      <c r="D6" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" t="s">
         <v>67</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G6">
-        <v>15</v>
-      </c>
       <c r="H6">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I6">
         <v>2</v>
       </c>
       <c r="J6">
-        <v>4</v>
-      </c>
-      <c r="K6" s="1">
+        <v>2</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+      <c r="L6" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="L6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M6" s="2" t="s">
+      <c r="N6" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6">
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q6">
         <v>1.4</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>93</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>1.3</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>89</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f>CONCATENATE(D7,"_lora-",F7,"_ebs-",H7*J7,"_lr-",K7,"-",L7)</f>
+        <f>CONCATENATE(E7,"_lora-",G7,"_ebs-",I7*K7,"_lr-",L7,"-",M7)</f>
         <v>bart-base_lora-8-32-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f>CONCATENATE(D7,"_uf-",E7,"_lora-",F7,"_nepoch-",G7,"_ebs-",H7*J7,"_lr-",K7,"-",L7,"_drop-",M7,"_wd-",N7)</f>
+        <f>CONCATENATE(E7,"_uf-",F7,"_lora-",G7,"_nepoch-",H7,"_ebs-",I7*K7,"_lr-",L7,"-",M7,"_drop-",N7,"_wd-",O7)</f>
         <v>bart-base_uf-none_lora-8-32-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D7" t="s">
-        <v>2</v>
+      <c r="D7" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E7" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" t="s">
         <v>67</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G7">
-        <v>15</v>
-      </c>
       <c r="H7">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I7">
         <v>2</v>
       </c>
       <c r="J7">
-        <v>4</v>
-      </c>
-      <c r="K7" s="1">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+      <c r="L7" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L7" s="2" t="s">
+      <c r="M7" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="N7" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7" t="s">
-        <v>6</v>
-      </c>
-      <c r="P7">
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q7">
         <v>1.3</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>1.2</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>89</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>CONCATENATE(D8,"_lora-",F8,"_ebs-",H8*J8,"_lr-",K8,"-",L8)</f>
+        <f>CONCATENATE(E8,"_lora-",G8,"_ebs-",I8*K8,"_lr-",L8,"-",M8)</f>
         <v>bart-base_lora-8-32-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>CONCATENATE(D8,"_uf-",E8,"_lora-",F8,"_nepoch-",G8,"_ebs-",H8*J8,"_lr-",K8,"-",L8,"_drop-",M8,"_wd-",N8)</f>
+        <f>CONCATENATE(E8,"_uf-",F8,"_lora-",G8,"_nepoch-",H8,"_ebs-",I8*K8,"_lr-",L8,"-",M8,"_drop-",N8,"_wd-",O8)</f>
         <v>bart-base_uf-none_lora-8-32-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D8" t="s">
-        <v>2</v>
+      <c r="D8" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E8" t="s">
+        <v>2</v>
+      </c>
+      <c r="F8" t="s">
         <v>67</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="G8">
-        <v>15</v>
-      </c>
       <c r="H8">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I8">
         <v>2</v>
       </c>
       <c r="J8">
-        <v>4</v>
-      </c>
-      <c r="K8" s="1">
+        <v>2</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+      <c r="L8" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L8" s="2" t="s">
+      <c r="M8" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M8" s="2" t="s">
+      <c r="N8" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N8">
-        <v>0</v>
-      </c>
-      <c r="O8" t="s">
-        <v>6</v>
-      </c>
-      <c r="P8">
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q8">
         <v>1.1299999999999999</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>1.2</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>89</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f>CONCATENATE(D9,"_lora-",F9,"_ebs-",H9*J9,"_lr-",K9,"-",L9)</f>
+        <f>CONCATENATE(E9,"_lora-",G9,"_ebs-",I9*K9,"_lr-",L9,"-",M9)</f>
         <v>bart-base_lora-32-32-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f>CONCATENATE(D9,"_uf-",E9,"_lora-",F9,"_nepoch-",G9,"_ebs-",H9*J9,"_lr-",K9,"-",L9,"_drop-",M9,"_wd-",N9)</f>
+        <f>CONCATENATE(E9,"_uf-",F9,"_lora-",G9,"_nepoch-",H9,"_ebs-",I9*K9,"_lr-",L9,"-",M9,"_drop-",N9,"_wd-",O9)</f>
         <v>bart-base_uf-none_lora-32-32-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D9" t="s">
-        <v>2</v>
+      <c r="D9" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
         <v>67</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="G9">
-        <v>15</v>
-      </c>
       <c r="H9">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I9">
         <v>2</v>
       </c>
       <c r="J9">
-        <v>4</v>
-      </c>
-      <c r="K9" s="1">
+        <v>2</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+      <c r="L9" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M9" s="2" t="s">
+      <c r="N9" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9">
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9">
         <v>1.3</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>1.2</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>89</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>CONCATENATE(D10,"_lora-",F10,"_ebs-",H10*J10,"_lr-",K10,"-",L10)</f>
+        <f>CONCATENATE(E10,"_lora-",G10,"_ebs-",I10*K10,"_lr-",L10,"-",M10)</f>
         <v>bart-base_lora-8-128-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f>CONCATENATE(D10,"_uf-",E10,"_lora-",F10,"_nepoch-",G10,"_ebs-",H10*J10,"_lr-",K10,"-",L10,"_drop-",M10,"_wd-",N10)</f>
+        <f>CONCATENATE(E10,"_uf-",F10,"_lora-",G10,"_nepoch-",H10,"_ebs-",I10*K10,"_lr-",L10,"-",M10,"_drop-",N10,"_wd-",O10)</f>
         <v>bart-base_uf-none_lora-8-128-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D10" t="s">
-        <v>2</v>
+      <c r="D10" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
         <v>67</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="G10">
-        <v>15</v>
-      </c>
       <c r="H10">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="J10">
-        <v>4</v>
-      </c>
-      <c r="K10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10">
+        <v>4</v>
+      </c>
+      <c r="L10" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M10" s="2" t="s">
+      <c r="N10" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N10">
-        <v>0</v>
-      </c>
-      <c r="O10" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10">
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10">
         <v>1.03</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>1.23</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>89</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f>CONCATENATE(D11,"_lora-",F11,"_ebs-",H11*J11,"_lr-",K11,"-",L11)</f>
+        <f>CONCATENATE(E11,"_lora-",G11,"_ebs-",I11*K11,"_lr-",L11,"-",M11)</f>
         <v>bart-base_lora-128-128-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C11" s="2" t="str">
-        <f>CONCATENATE(D11,"_uf-",E11,"_lora-",F11,"_nepoch-",G11,"_ebs-",H11*J11,"_lr-",K11,"-",L11,"_drop-",M11,"_wd-",N11)</f>
+        <f>CONCATENATE(E11,"_uf-",F11,"_lora-",G11,"_nepoch-",H11,"_ebs-",I11*K11,"_lr-",L11,"-",M11,"_drop-",N11,"_wd-",O11)</f>
         <v>bart-base_uf-none_lora-128-128-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D11" t="s">
-        <v>2</v>
+      <c r="D11" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="G11">
-        <v>15</v>
-      </c>
       <c r="H11">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="J11">
-        <v>4</v>
-      </c>
-      <c r="K11" s="1">
+        <v>2</v>
+      </c>
+      <c r="K11">
+        <v>4</v>
+      </c>
+      <c r="L11" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="N11" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11" t="s">
-        <v>6</v>
-      </c>
-      <c r="P11">
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q11">
         <v>0.77</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>93</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>1.26</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>89</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>CONCATENATE(D12,"_lora-",F12,"_ebs-",H12*J12,"_lr-",K12,"-",L12)</f>
+        <f>CONCATENATE(E12,"_lora-",G12,"_ebs-",I12*K12,"_lr-",L12,"-",M12)</f>
         <v>bart-base_lora-512-128-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C12" s="2" t="str">
-        <f>CONCATENATE(D12,"_uf-",E12,"_lora-",F12,"_nepoch-",G12,"_ebs-",H12*J12,"_lr-",K12,"-",L12,"_drop-",M12,"_wd-",N12)</f>
+        <f>CONCATENATE(E12,"_uf-",F12,"_lora-",G12,"_nepoch-",H12,"_ebs-",I12*K12,"_lr-",L12,"-",M12,"_drop-",N12,"_wd-",O12)</f>
         <v>bart-base_uf-none_lora-512-128-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D12" t="s">
-        <v>2</v>
+      <c r="D12" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G12">
-        <v>15</v>
-      </c>
       <c r="H12">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I12">
         <v>2</v>
       </c>
       <c r="J12">
-        <v>4</v>
-      </c>
-      <c r="K12" s="1">
+        <v>2</v>
+      </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
+      <c r="L12" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M12" s="2" t="s">
+      <c r="N12" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-      <c r="O12" t="s">
-        <v>6</v>
-      </c>
-      <c r="P12">
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q12">
         <v>0.8</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>1.24</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>89</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f>CONCATENATE(D13,"_lora-",F13,"_ebs-",H13*J13,"_lr-",K13,"-",L13)</f>
+        <f>CONCATENATE(E13,"_lora-",G13,"_ebs-",I13*K13,"_lr-",L13,"-",M13)</f>
         <v>bart-base_lora-512-128-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f>CONCATENATE(D13,"_uf-",E13,"_lora-",F13,"_nepoch-",G13,"_ebs-",H13*J13,"_lr-",K13,"-",L13,"_drop-",M13,"_wd-",N13)</f>
+        <f>CONCATENATE(E13,"_uf-",F13,"_lora-",G13,"_nepoch-",H13,"_ebs-",I13*K13,"_lr-",L13,"-",M13,"_drop-",N13,"_wd-",O13)</f>
         <v>bart-base_uf-none_lora-512-128-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D13" t="s">
-        <v>2</v>
+      <c r="D13" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E13" t="s">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G13">
-        <v>15</v>
-      </c>
       <c r="H13">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
       <c r="J13">
-        <v>4</v>
-      </c>
-      <c r="K13" s="1">
+        <v>2</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+      <c r="L13" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M13" s="2" t="s">
+      <c r="N13" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N13">
-        <v>0</v>
-      </c>
-      <c r="O13" t="s">
-        <v>6</v>
-      </c>
-      <c r="P13">
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q13">
         <v>1</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>1.2</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>89</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f>CONCATENATE(D14,"_lora-",F14,"_ebs-",H14*J14,"_lr-",K14,"-",L14)</f>
+        <f>CONCATENATE(E14,"_lora-",G14,"_ebs-",I14*K14,"_lr-",L14,"-",M14)</f>
         <v>bart-base_lora-512-128-0_ebs-8_lr-0.0032-step-1-0.998</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f>CONCATENATE(D14,"_uf-",E14,"_lora-",F14,"_nepoch-",G14,"_ebs-",H14*J14,"_lr-",K14,"-",L14,"_drop-",M14,"_wd-",N14)</f>
+        <f>CONCATENATE(E14,"_uf-",F14,"_lora-",G14,"_nepoch-",H14,"_ebs-",I14*K14,"_lr-",L14,"-",M14,"_drop-",N14,"_wd-",O14)</f>
         <v>bart-base_uf-none_lora-512-128-0_nepoch-15_ebs-8_lr-0.0032-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D14" t="s">
-        <v>2</v>
+      <c r="D14" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="G14">
-        <v>15</v>
-      </c>
       <c r="H14">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I14">
         <v>2</v>
       </c>
       <c r="J14">
-        <v>4</v>
-      </c>
-      <c r="K14" s="1">
+        <v>2</v>
+      </c>
+      <c r="K14">
+        <v>4</v>
+      </c>
+      <c r="L14" s="1">
         <v>3.2000000000000002E-3</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M14" s="2" t="s">
+      <c r="N14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N14">
-        <v>0</v>
-      </c>
-      <c r="O14" t="s">
-        <v>6</v>
-      </c>
-      <c r="P14">
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q14">
         <v>0.8</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>1.33</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>89</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f>CONCATENATE(D15,"_lora-",F15,"_ebs-",H15*J15,"_lr-",K15,"-",L15)</f>
+        <f>CONCATENATE(E15,"_lora-",G15,"_ebs-",I15*K15,"_lr-",L15,"-",M15)</f>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f>CONCATENATE(D15,"_uf-",E15,"_lora-",F15,"_nepoch-",G15,"_ebs-",H15*J15,"_lr-",K15,"-",L15,"_drop-",M15,"_wd-",N15)</f>
+        <f>CONCATENATE(E15,"_uf-",F15,"_lora-",G15,"_nepoch-",H15,"_ebs-",I15*K15,"_lr-",L15,"-",M15,"_drop-",N15,"_wd-",O15)</f>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D15" t="s">
-        <v>2</v>
+      <c r="D15" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F15" t="s">
         <v>67</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G15">
-        <v>15</v>
-      </c>
       <c r="H15">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I15">
         <v>2</v>
       </c>
       <c r="J15">
-        <v>4</v>
-      </c>
-      <c r="K15" s="1">
+        <v>2</v>
+      </c>
+      <c r="K15">
+        <v>4</v>
+      </c>
+      <c r="L15" s="1">
         <v>1.6000000000000001E-3</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M15" s="2" t="s">
+      <c r="N15" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N15">
-        <v>0</v>
-      </c>
-      <c r="O15" t="s">
-        <v>6</v>
-      </c>
-      <c r="P15">
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q15">
         <v>0.7</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>1.4</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>89</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f>CONCATENATE(D16,"_lora-",F16,"_ebs-",H16*J16,"_lr-",K16,"-",L16)</f>
+        <f>CONCATENATE(E16,"_lora-",G16,"_ebs-",I16*K16,"_lr-",L16,"-",M16)</f>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f>CONCATENATE(D16,"_uf-",E16,"_lora-",F16,"_nepoch-",G16,"_ebs-",H16*J16,"_lr-",K16,"-",L16,"_drop-",M16,"_wd-",N16)</f>
+        <f>CONCATENATE(E16,"_uf-",F16,"_lora-",G16,"_nepoch-",H16,"_ebs-",I16*K16,"_lr-",L16,"-",M16,"_drop-",N16,"_wd-",O16)</f>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D16" t="s">
-        <v>2</v>
+      <c r="D16" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E16" t="s">
+        <v>2</v>
+      </c>
+      <c r="F16" t="s">
         <v>67</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G16">
-        <v>15</v>
-      </c>
       <c r="H16">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I16">
         <v>2</v>
       </c>
       <c r="J16">
-        <v>4</v>
-      </c>
-      <c r="K16" s="1">
+        <v>2</v>
+      </c>
+      <c r="K16">
+        <v>4</v>
+      </c>
+      <c r="L16" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L16" s="2" t="s">
+      <c r="M16" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M16" s="2" t="s">
+      <c r="N16" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N16">
-        <v>0</v>
-      </c>
-      <c r="O16" t="s">
-        <v>6</v>
-      </c>
-      <c r="P16">
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q16">
         <v>0.64</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>1.3</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>89</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f>CONCATENATE(D17,"_lora-",F17,"_ebs-",H17*J17,"_lr-",K17,"-",L17)</f>
+        <f>CONCATENATE(E17,"_lora-",G17,"_ebs-",I17*K17,"_lr-",L17,"-",M17)</f>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0004-step-1-0.998</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f>CONCATENATE(D17,"_uf-",E17,"_lora-",F17,"_nepoch-",G17,"_ebs-",H17*J17,"_lr-",K17,"-",L17,"_drop-",M17,"_wd-",N17)</f>
+        <f>CONCATENATE(E17,"_uf-",F17,"_lora-",G17,"_nepoch-",H17,"_ebs-",I17*K17,"_lr-",L17,"-",M17,"_drop-",N17,"_wd-",O17)</f>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D17" t="s">
-        <v>2</v>
+      <c r="D17" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
         <v>67</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G17">
-        <v>15</v>
-      </c>
       <c r="H17">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I17">
         <v>2</v>
       </c>
       <c r="J17">
-        <v>4</v>
-      </c>
-      <c r="K17" s="1">
+        <v>2</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+      <c r="L17" s="1">
         <v>4.0000000000000002E-4</v>
       </c>
-      <c r="L17" s="2" t="s">
+      <c r="M17" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="M17" s="2" t="s">
+      <c r="N17" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N17">
-        <v>0</v>
-      </c>
-      <c r="O17" t="s">
-        <v>6</v>
-      </c>
-      <c r="P17">
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17">
         <v>0.9</v>
       </c>
-      <c r="R17">
+      <c r="S17">
         <v>1.2</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>89</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f>CONCATENATE(D18,"_lora-",F18,"_ebs-",H18*J18,"_lr-",K18,"-",L18)</f>
+        <f>CONCATENATE(E18,"_lora-",G18,"_ebs-",I18*K18,"_lr-",L18,"-",M18)</f>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.997</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f>CONCATENATE(D18,"_uf-",E18,"_lora-",F18,"_nepoch-",G18,"_ebs-",H18*J18,"_lr-",K18,"-",L18,"_drop-",M18,"_wd-",N18)</f>
+        <f>CONCATENATE(E18,"_uf-",F18,"_lora-",G18,"_nepoch-",H18,"_ebs-",I18*K18,"_lr-",L18,"-",M18,"_drop-",N18,"_wd-",O18)</f>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.997_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D18" t="s">
-        <v>2</v>
+      <c r="D18" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E18" t="s">
+        <v>2</v>
+      </c>
+      <c r="F18" t="s">
         <v>67</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="G18" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G18">
-        <v>15</v>
-      </c>
       <c r="H18">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I18">
         <v>2</v>
       </c>
       <c r="J18">
-        <v>4</v>
-      </c>
-      <c r="K18" s="1">
+        <v>2</v>
+      </c>
+      <c r="K18">
+        <v>4</v>
+      </c>
+      <c r="L18" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L18" s="2" t="s">
+      <c r="M18" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="M18" s="2" t="s">
+      <c r="N18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
-      <c r="O18" t="s">
-        <v>6</v>
-      </c>
-      <c r="P18">
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q18">
         <v>0.83</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>1.23</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>89</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f>CONCATENATE(D19,"_lora-",F19,"_ebs-",H19*J19,"_lr-",K19,"-",L19)</f>
+        <f>CONCATENATE(E19,"_lora-",G19,"_ebs-",I19*K19,"_lr-",L19,"-",M19)</f>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f>CONCATENATE(D19,"_uf-",E19,"_lora-",F19,"_nepoch-",G19,"_ebs-",H19*J19,"_lr-",K19,"-",L19,"_drop-",M19,"_wd-",N19)</f>
+        <f>CONCATENATE(E19,"_uf-",F19,"_lora-",G19,"_nepoch-",H19,"_ebs-",I19*K19,"_lr-",L19,"-",M19,"_drop-",N19,"_wd-",O19)</f>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D19" t="s">
-        <v>2</v>
+      <c r="D19" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E19" t="s">
+        <v>2</v>
+      </c>
+      <c r="F19" t="s">
         <v>67</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G19">
-        <v>15</v>
-      </c>
       <c r="H19">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="I19">
         <v>2</v>
       </c>
       <c r="J19">
-        <v>4</v>
-      </c>
-      <c r="K19" s="1">
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <v>4</v>
+      </c>
+      <c r="L19" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L19" s="2" t="s">
+      <c r="M19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M19" s="2" t="s">
+      <c r="N19" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N19">
-        <v>0</v>
-      </c>
-      <c r="O19" t="s">
-        <v>6</v>
-      </c>
-      <c r="P19">
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19">
         <v>0.52</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>109</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>1.37</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>89</v>
       </c>
       <c r="B20" s="2" t="str">
-        <f>CONCATENATE(D20,"_lora-",F20,"_ebs-",H20*J20,"_lr-",K20,"-",L20,"_pt2")</f>
+        <f>CONCATENATE(E20,"_lora-",G20,"_ebs-",I20*K20,"_lr-",L20,"-",M20,"_pt2")</f>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f>CONCATENATE(D20,"_uf-",E20,"_lora-",F20,"_nepoch-",G20,"_ebs-",H20*J20,"_lr-",K20,"-",L20,"_drop-",M20,"_wd-",N20)</f>
+        <f>CONCATENATE(E20,"_uf-",F20,"_lora-",G20,"_nepoch-",H20,"_ebs-",I20*K20,"_lr-",L20,"-",M20,"_drop-",N20,"_wd-",O20)</f>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-30_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
       </c>
-      <c r="D20" t="s">
-        <v>2</v>
+      <c r="D20" s="2" t="s">
+        <v>115</v>
       </c>
       <c r="E20" t="s">
+        <v>2</v>
+      </c>
+      <c r="F20" t="s">
         <v>67</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="G20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>30</v>
       </c>
-      <c r="H20">
-        <v>2</v>
-      </c>
       <c r="I20">
         <v>2</v>
       </c>
       <c r="J20">
-        <v>4</v>
-      </c>
-      <c r="K20" s="1">
+        <v>2</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+      <c r="L20" s="1">
         <v>8.0000000000000004E-4</v>
       </c>
-      <c r="L20" s="2" t="s">
+      <c r="M20" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="M20" s="2" t="s">
+      <c r="N20" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20" t="s">
-        <v>6</v>
-      </c>
-      <c r="P20">
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q20">
         <v>0.3</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>110</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>1.5</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>103</v>
       </c>
     </row>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="2" t="str">
+        <f>CONCATENATE(E21,"_lora-",G21,"_ebs-",I21*K21,"_lr-",L21,"-",M21)</f>
+        <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.9992</v>
+      </c>
+      <c r="C21" s="2" t="str">
+        <f>CONCATENATE(E21,"_uf-",F21,"_lora-",G21,"_nepoch-",H21,"_ebs-",I21*K21,"_lr-",L21,"-",M21,"_drop-",N21,"_wd-",O21)</f>
+        <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.9992_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E21" t="s">
+        <v>2</v>
+      </c>
+      <c r="F21" t="s">
+        <v>67</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H21">
+        <v>15</v>
+      </c>
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <v>2</v>
+      </c>
+      <c r="K21">
+        <v>4</v>
+      </c>
+      <c r="L21" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O21">
+        <v>0</v>
+      </c>
+      <c r="P21" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q21">
+        <v>0.48</v>
+      </c>
+      <c r="S21">
+        <v>1.52</v>
+      </c>
+      <c r="T21" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="2" t="str">
+        <f>CONCATENATE(E22,"_lora-",G22,"_ebs-",I22*K22,"_lr-",L22,"-",M22)</f>
+        <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.9994</v>
+      </c>
+      <c r="C22" s="2" t="str">
+        <f>CONCATENATE(E22,"_uf-",F22,"_lora-",G22,"_nepoch-",H22,"_ebs-",I22*K22,"_lr-",L22,"-",M22,"_drop-",N22,"_wd-",O22)</f>
+        <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.9994_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>67</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H22">
+        <v>15</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>2</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="2" t="str">
+        <f>CONCATENATE(E23,"_uf-",F23,"_ebs-",I23*K23,"_lr-",L23,"-",M23,"_",D23)</f>
+        <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_ogtvsplit</v>
+      </c>
+      <c r="C23" s="2" t="str">
+        <f>CONCATENATE(E23,"_uf-",F23,"_lora-",G23,"_nepoch-",H23,"_ebs-",I23*K23,"_lr-",L23,"-",M23,"_drop-",N23,"_wd-",O23)</f>
+        <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>79</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H23">
+        <v>15</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>2</v>
+      </c>
+      <c r="K23">
+        <v>4</v>
+      </c>
+      <c r="L23" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N23" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="2" t="str">
+        <f>CONCATENATE(E24,"_lora-",G24,"_ebs-",I24*K24,"_lr-",L24,"-",M24,"_",D24)</f>
+        <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_ogtvsplit</v>
+      </c>
+      <c r="C24" s="2" t="str">
+        <f>CONCATENATE(E24,"_uf-",F24,"_lora-",G24,"_nepoch-",H24,"_ebs-",I24*K24,"_lr-",L24,"-",M24,"_drop-",N24,"_wd-",O24)</f>
+        <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="H24">
+        <v>15</v>
+      </c>
+      <c r="I24">
+        <v>2</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24" s="1">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="N24" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:S1" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}"/>
+  <autoFilter ref="A1:T1" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
text_summ: finished running inference on training and validation data for models to sanity-check performance
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E70356F9-C959-42B2-81ED-2CF5E06C5CB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9430352-F9A6-4337-A875-B6A9EB79D9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="logs-1" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="logs" sheetId="3" r:id="rId2"/>
+    <sheet name="rouge" sheetId="9" r:id="rId3"/>
+    <sheet name="bertscore" sheetId="10" r:id="rId4"/>
+    <sheet name="predictions" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">logs!$A$1:$T$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'logs-1'!$A$1:$Q$102</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet1!$A$1:$T$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="138">
   <si>
     <t>Log ID</t>
   </si>
@@ -395,6 +398,69 @@
   </si>
   <si>
     <t>Use original dataset</t>
+  </si>
+  <si>
+    <t>log id</t>
+  </si>
+  <si>
+    <t>train_loss</t>
+  </si>
+  <si>
+    <t>train_bertscore_precision</t>
+  </si>
+  <si>
+    <t>train_bertscore_recall</t>
+  </si>
+  <si>
+    <t>train_bertscore_f1</t>
+  </si>
+  <si>
+    <t>train_rouge1</t>
+  </si>
+  <si>
+    <t>train_rouge2</t>
+  </si>
+  <si>
+    <t>train_rougeL</t>
+  </si>
+  <si>
+    <t>train_rougeLsum</t>
+  </si>
+  <si>
+    <t>val_loss</t>
+  </si>
+  <si>
+    <t>val_bertscore_precision</t>
+  </si>
+  <si>
+    <t>val_bertscore_recall</t>
+  </si>
+  <si>
+    <t>val_bertscore_f1</t>
+  </si>
+  <si>
+    <t>val_rouge1</t>
+  </si>
+  <si>
+    <t>val_rouge2</t>
+  </si>
+  <si>
+    <t>val_rougeL</t>
+  </si>
+  <si>
+    <t>val_rougeLsum</t>
+  </si>
+  <si>
+    <t>har1</t>
+  </si>
+  <si>
+    <t>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_ogtvsplit_checkpoint-2250</t>
+  </si>
+  <si>
+    <t>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_checkpoint-1950</t>
+  </si>
+  <si>
+    <t>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2_checkpoint-3900</t>
   </si>
 </sst>
 </file>
@@ -452,6 +518,2377 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>har1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>train_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>train_rougeLsum</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>val_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>val_rougeLsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.58613999548213402</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.43225905001142201</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.52669642999034105</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.56701136296431898</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.542185131871735</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.338884305700136</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.46344538742345798</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.51276177045692595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6007-4FF2-923B-91A4F8965DBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_ogtvsplit_checkpoint-2250</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>train_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>train_rougeLsum</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>val_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>val_rougeLsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.97748907382345296</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96961754966096103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97448815186620796</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97652762803676996</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.63930569693966999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.475385897569164</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.57557190558245097</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.61692626988087296</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-6007-4FF2-923B-91A4F8965DBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_checkpoint-1950</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>train_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>train_rougeLsum</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>val_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>val_rougeLsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.98716446702413396</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98128093172282405</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98522155850655102</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.98662197894697101</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.64662630601860704</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.52131505379659304</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.60460040299245199</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.62844741599200604</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-6007-4FF2-923B-91A4F8965DBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2_checkpoint-3900</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$2:$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>train_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>train_rougeLsum</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_rouge1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_rouge2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>val_rougeL</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>val_rougeLsum</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0.914446934937589</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.87164045647703103</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.90066514133917996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90842865118018501</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.67565411551627297</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.54618426545592003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.62727284115202497</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.65661235587094802</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-6007-4FF2-923B-91A4F8965DBD}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="503402624"/>
+        <c:axId val="503402144"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="503402624"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503402144"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="503402144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="503402624"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>har1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$10:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>train_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_bertscore_f1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>val_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_bertscore_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$B$10:$B$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.87178488065798998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91668640504280696</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89280132864912298</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.86903984665870604</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.910506426095962</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.88882164955139098</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-279A-4CFE-A777-B620C8089828}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_ogtvsplit_checkpoint-2250</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$10:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>train_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_bertscore_f1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>val_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_bertscore_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$C$10:$C$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.99285753900806095</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.98422385394573197</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.98839561864733605</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91628366470336897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89144927024841303</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90296375930309203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-279A-4CFE-A777-B620C8089828}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_checkpoint-1950</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$10:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>train_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_bertscore_f1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>val_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_bertscore_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$D$10:$D$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.99486780567810995</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.99189906957057805</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.99332246442253702</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90856541331970297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88854957033287396</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.89712021341829495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-279A-4CFE-A777-B620C8089828}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>predictions!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2_checkpoint-3900</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>predictions!$A$10:$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>train_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>train_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>train_bertscore_f1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>val_bertscore_precision</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>val_bertscore_recall</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>val_bertscore_f1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>predictions!$E$10:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0.97916563308009696</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96298882072934699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97078474066578402</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.92143840816887901</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89527373286810696</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.90697302014538705</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-279A-4CFE-A777-B620C8089828}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="524620272"/>
+        <c:axId val="524622192"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="524620272"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524622192"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="524622192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="524620272"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/chartsheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1C54EF21-B404-48C9-B75B-1BFB5F9FE0C7}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/chartsheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7C849BBB-4DC5-45E0-BCB8-5778C27377E3}">
+  <sheetPr/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+  </sheetViews>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</chartsheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8675165" cy="6296766"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F6E6AB3-56EA-FB5E-CBBA-278FECD42C3F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:absoluteAnchor>
+    <xdr:pos x="0" y="0"/>
+    <xdr:ext cx="8675165" cy="6296766"/>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D548DD1E-6A08-B73A-1DB7-C1DFA6476D28}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks noGrp="1"/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:absoluteAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -775,7 +3212,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D37" sqref="D37"/>
+      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3906,9 +6343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4005,7 +6442,7 @@
         <v>bart-base_uf-all_ebs-8_lr-0.00005-step-1-0.998</v>
       </c>
       <c r="C2" s="2" t="str">
-        <f>CONCATENATE(E2,"_uf-",F2,"_lora-",G2,"_nepoch-",H2,"_ebs-",I2*K2,"_lr-",L2,"-",M2,"_drop-",N2,"_wd-",O2)</f>
+        <f t="shared" ref="C2:C24" si="0">CONCATENATE(E2,"_uf-",F2,"_lora-",G2,"_nepoch-",H2,"_ebs-",I2*K2,"_lr-",L2,"-",M2,"_drop-",N2,"_wd-",O2)</f>
         <v>bart-base_uf-all_lora-none_nepoch-30_ebs-8_lr-0.00005-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D2" s="2" t="s">
@@ -4062,11 +6499,11 @@
         <v>87</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B4" si="0">CONCATENATE(E3,"_uf-",F3,"_ebs-",I3*K3,"_lr-",L3,"-",M3)</f>
+        <f t="shared" ref="B3:B4" si="1">CONCATENATE(E3,"_uf-",F3,"_ebs-",I3*K3,"_lr-",L3,"-",M3)</f>
         <v>bart-base_uf-all_ebs-8_lr-0.0001-step-1-0.998</v>
       </c>
       <c r="C3" s="2" t="str">
-        <f>CONCATENATE(E3,"_uf-",F3,"_lora-",G3,"_nepoch-",H3,"_ebs-",I3*K3,"_lr-",L3,"-",M3,"_drop-",N3,"_wd-",O3)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0001-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -4126,11 +6563,11 @@
         <v>87</v>
       </c>
       <c r="B4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>bart-base_uf-all_ebs-8_lr-0.0002-step-1-0.998</v>
+      </c>
+      <c r="C4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>bart-base_uf-all_ebs-8_lr-0.0002-step-1-0.998</v>
-      </c>
-      <c r="C4" s="2" t="str">
-        <f>CONCATENATE(E4,"_uf-",F4,"_lora-",G4,"_nepoch-",H4,"_ebs-",I4*K4,"_lr-",L4,"-",M4,"_drop-",N4,"_wd-",O4)</f>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0002-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D4" s="2" t="s">
@@ -4190,11 +6627,11 @@
         <v>87</v>
       </c>
       <c r="B5" s="2" t="str">
-        <f t="shared" ref="B5" si="1">CONCATENATE(E5,"_uf-",F5,"_ebs-",I5*K5,"_lr-",L5,"-",M5)</f>
+        <f t="shared" ref="B5" si="2">CONCATENATE(E5,"_uf-",F5,"_ebs-",I5*K5,"_lr-",L5,"-",M5)</f>
         <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998</v>
       </c>
       <c r="C5" s="2" t="str">
-        <f>CONCATENATE(E5,"_uf-",F5,"_lora-",G5,"_nepoch-",H5,"_ebs-",I5*K5,"_lr-",L5,"-",M5,"_drop-",N5,"_wd-",O5)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D5" s="2" t="s">
@@ -4254,11 +6691,11 @@
         <v>89</v>
       </c>
       <c r="B6" s="2" t="str">
-        <f>CONCATENATE(E6,"_lora-",G6,"_ebs-",I6*K6,"_lr-",L6,"-",M6)</f>
+        <f t="shared" ref="B6:B19" si="3">CONCATENATE(E6,"_lora-",G6,"_ebs-",I6*K6,"_lr-",L6,"-",M6)</f>
         <v>bart-base_lora-8-32-0_ebs-8_lr-0.0004-step-1-0.998</v>
       </c>
       <c r="C6" s="2" t="str">
-        <f>CONCATENATE(E6,"_uf-",F6,"_lora-",G6,"_nepoch-",H6,"_ebs-",I6*K6,"_lr-",L6,"-",M6,"_drop-",N6,"_wd-",O6)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-8-32-0_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D6" s="2" t="s">
@@ -4318,11 +6755,11 @@
         <v>89</v>
       </c>
       <c r="B7" s="2" t="str">
-        <f>CONCATENATE(E7,"_lora-",G7,"_ebs-",I7*K7,"_lr-",L7,"-",M7)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-8-32-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C7" s="2" t="str">
-        <f>CONCATENATE(E7,"_uf-",F7,"_lora-",G7,"_nepoch-",H7,"_ebs-",I7*K7,"_lr-",L7,"-",M7,"_drop-",N7,"_wd-",O7)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-8-32-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D7" s="2" t="s">
@@ -4379,11 +6816,11 @@
         <v>89</v>
       </c>
       <c r="B8" s="2" t="str">
-        <f>CONCATENATE(E8,"_lora-",G8,"_ebs-",I8*K8,"_lr-",L8,"-",M8)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-8-32-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C8" s="2" t="str">
-        <f>CONCATENATE(E8,"_uf-",F8,"_lora-",G8,"_nepoch-",H8,"_ebs-",I8*K8,"_lr-",L8,"-",M8,"_drop-",N8,"_wd-",O8)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-8-32-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D8" s="2" t="s">
@@ -4440,11 +6877,11 @@
         <v>89</v>
       </c>
       <c r="B9" s="2" t="str">
-        <f>CONCATENATE(E9,"_lora-",G9,"_ebs-",I9*K9,"_lr-",L9,"-",M9)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-32-32-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C9" s="2" t="str">
-        <f>CONCATENATE(E9,"_uf-",F9,"_lora-",G9,"_nepoch-",H9,"_ebs-",I9*K9,"_lr-",L9,"-",M9,"_drop-",N9,"_wd-",O9)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-32-32-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D9" s="2" t="s">
@@ -4501,11 +6938,11 @@
         <v>89</v>
       </c>
       <c r="B10" s="2" t="str">
-        <f>CONCATENATE(E10,"_lora-",G10,"_ebs-",I10*K10,"_lr-",L10,"-",M10)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-8-128-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C10" s="2" t="str">
-        <f>CONCATENATE(E10,"_uf-",F10,"_lora-",G10,"_nepoch-",H10,"_ebs-",I10*K10,"_lr-",L10,"-",M10,"_drop-",N10,"_wd-",O10)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-8-128-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D10" s="2" t="s">
@@ -4562,11 +6999,11 @@
         <v>89</v>
       </c>
       <c r="B11" s="2" t="str">
-        <f>CONCATENATE(E11,"_lora-",G11,"_ebs-",I11*K11,"_lr-",L11,"-",M11)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-128-128-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C11" s="2" t="str">
-        <f>CONCATENATE(E11,"_uf-",F11,"_lora-",G11,"_nepoch-",H11,"_ebs-",I11*K11,"_lr-",L11,"-",M11,"_drop-",N11,"_wd-",O11)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-128-128-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D11" s="2" t="s">
@@ -4626,11 +7063,11 @@
         <v>89</v>
       </c>
       <c r="B12" s="2" t="str">
-        <f>CONCATENATE(E12,"_lora-",G12,"_ebs-",I12*K12,"_lr-",L12,"-",M12)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-128-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C12" s="2" t="str">
-        <f>CONCATENATE(E12,"_uf-",F12,"_lora-",G12,"_nepoch-",H12,"_ebs-",I12*K12,"_lr-",L12,"-",M12,"_drop-",N12,"_wd-",O12)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-128-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D12" s="2" t="s">
@@ -4687,11 +7124,11 @@
         <v>89</v>
       </c>
       <c r="B13" s="2" t="str">
-        <f>CONCATENATE(E13,"_lora-",G13,"_ebs-",I13*K13,"_lr-",L13,"-",M13)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-128-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C13" s="2" t="str">
-        <f>CONCATENATE(E13,"_uf-",F13,"_lora-",G13,"_nepoch-",H13,"_ebs-",I13*K13,"_lr-",L13,"-",M13,"_drop-",N13,"_wd-",O13)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-128-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D13" s="2" t="s">
@@ -4748,11 +7185,11 @@
         <v>89</v>
       </c>
       <c r="B14" s="2" t="str">
-        <f>CONCATENATE(E14,"_lora-",G14,"_ebs-",I14*K14,"_lr-",L14,"-",M14)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-128-0_ebs-8_lr-0.0032-step-1-0.998</v>
       </c>
       <c r="C14" s="2" t="str">
-        <f>CONCATENATE(E14,"_uf-",F14,"_lora-",G14,"_nepoch-",H14,"_ebs-",I14*K14,"_lr-",L14,"-",M14,"_drop-",N14,"_wd-",O14)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-128-0_nepoch-15_ebs-8_lr-0.0032-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D14" s="2" t="s">
@@ -4809,11 +7246,11 @@
         <v>89</v>
       </c>
       <c r="B15" s="2" t="str">
-        <f>CONCATENATE(E15,"_lora-",G15,"_ebs-",I15*K15,"_lr-",L15,"-",M15)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0016-step-1-0.998</v>
       </c>
       <c r="C15" s="2" t="str">
-        <f>CONCATENATE(E15,"_uf-",F15,"_lora-",G15,"_nepoch-",H15,"_ebs-",I15*K15,"_lr-",L15,"-",M15,"_drop-",N15,"_wd-",O15)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0016-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D15" s="2" t="s">
@@ -4870,11 +7307,11 @@
         <v>89</v>
       </c>
       <c r="B16" s="2" t="str">
-        <f>CONCATENATE(E16,"_lora-",G16,"_ebs-",I16*K16,"_lr-",L16,"-",M16)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.998</v>
       </c>
       <c r="C16" s="2" t="str">
-        <f>CONCATENATE(E16,"_uf-",F16,"_lora-",G16,"_nepoch-",H16,"_ebs-",I16*K16,"_lr-",L16,"-",M16,"_drop-",N16,"_wd-",O16)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D16" s="2" t="s">
@@ -4931,11 +7368,11 @@
         <v>89</v>
       </c>
       <c r="B17" s="2" t="str">
-        <f>CONCATENATE(E17,"_lora-",G17,"_ebs-",I17*K17,"_lr-",L17,"-",M17)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0004-step-1-0.998</v>
       </c>
       <c r="C17" s="2" t="str">
-        <f>CONCATENATE(E17,"_uf-",F17,"_lora-",G17,"_nepoch-",H17,"_ebs-",I17*K17,"_lr-",L17,"-",M17,"_drop-",N17,"_wd-",O17)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -4992,11 +7429,11 @@
         <v>89</v>
       </c>
       <c r="B18" s="2" t="str">
-        <f>CONCATENATE(E18,"_lora-",G18,"_ebs-",I18*K18,"_lr-",L18,"-",M18)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.997</v>
       </c>
       <c r="C18" s="2" t="str">
-        <f>CONCATENATE(E18,"_uf-",F18,"_lora-",G18,"_nepoch-",H18,"_ebs-",I18*K18,"_lr-",L18,"-",M18,"_drop-",N18,"_wd-",O18)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.997_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -5053,11 +7490,11 @@
         <v>89</v>
       </c>
       <c r="B19" s="2" t="str">
-        <f>CONCATENATE(E19,"_lora-",G19,"_ebs-",I19*K19,"_lr-",L19,"-",M19)</f>
+        <f t="shared" si="3"/>
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999</v>
       </c>
       <c r="C19" s="2" t="str">
-        <f>CONCATENATE(E19,"_uf-",F19,"_lora-",G19,"_nepoch-",H19,"_ebs-",I19*K19,"_lr-",L19,"-",M19,"_drop-",N19,"_wd-",O19)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D19" s="2" t="s">
@@ -5121,7 +7558,7 @@
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2</v>
       </c>
       <c r="C20" s="2" t="str">
-        <f>CONCATENATE(E20,"_uf-",F20,"_lora-",G20,"_nepoch-",H20,"_ebs-",I20*K20,"_lr-",L20,"-",M20,"_drop-",N20,"_wd-",O20)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-30_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D20" s="2" t="s">
@@ -5185,7 +7622,7 @@
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.9992</v>
       </c>
       <c r="C21" s="2" t="str">
-        <f>CONCATENATE(E21,"_uf-",F21,"_lora-",G21,"_nepoch-",H21,"_ebs-",I21*K21,"_lr-",L21,"-",M21,"_drop-",N21,"_wd-",O21)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.9992_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D21" s="2" t="s">
@@ -5246,7 +7683,7 @@
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.9994</v>
       </c>
       <c r="C22" s="2" t="str">
-        <f>CONCATENATE(E22,"_uf-",F22,"_lora-",G22,"_nepoch-",H22,"_ebs-",I22*K22,"_lr-",L22,"-",M22,"_drop-",N22,"_wd-",O22)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.9994_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D22" s="2" t="s">
@@ -5298,7 +7735,7 @@
         <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_ogtvsplit</v>
       </c>
       <c r="C23" s="2" t="str">
-        <f>CONCATENATE(E23,"_uf-",F23,"_lora-",G23,"_nepoch-",H23,"_ebs-",I23*K23,"_lr-",L23,"-",M23,"_drop-",N23,"_wd-",O23)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D23" s="2" t="s">
@@ -5350,7 +7787,7 @@
         <v>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_ogtvsplit</v>
       </c>
       <c r="C24" s="2" t="str">
-        <f>CONCATENATE(E24,"_uf-",F24,"_lora-",G24,"_nepoch-",H24,"_ebs-",I24*K24,"_lr-",L24,"-",M24,"_drop-",N24,"_wd-",O24)</f>
+        <f t="shared" si="0"/>
         <v>bart-base_uf-none_lora-512-512-0_nepoch-15_ebs-8_lr-0.0008-step-1-0.999_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D24" s="2" t="s">
@@ -5397,4 +7834,309 @@
   <autoFilter ref="A1:T1" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2A54BE6-A7EA-4CDA-934F-71CDBC139798}">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" activeCellId="1" sqref="A1:E1 A10:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" customWidth="1"/>
+    <col min="3" max="3" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="73.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="69.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2">
+        <v>0.58613999548213402</v>
+      </c>
+      <c r="C2">
+        <v>0.97748907382345296</v>
+      </c>
+      <c r="D2">
+        <v>0.98716446702413396</v>
+      </c>
+      <c r="E2">
+        <v>0.914446934937589</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3">
+        <v>0.43225905001142201</v>
+      </c>
+      <c r="C3">
+        <v>0.96961754966096103</v>
+      </c>
+      <c r="D3">
+        <v>0.98128093172282405</v>
+      </c>
+      <c r="E3">
+        <v>0.87164045647703103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4">
+        <v>0.52669642999034105</v>
+      </c>
+      <c r="C4">
+        <v>0.97448815186620796</v>
+      </c>
+      <c r="D4">
+        <v>0.98522155850655102</v>
+      </c>
+      <c r="E4">
+        <v>0.90066514133917996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5">
+        <v>0.56701136296431898</v>
+      </c>
+      <c r="C5">
+        <v>0.97652762803676996</v>
+      </c>
+      <c r="D5">
+        <v>0.98662197894697101</v>
+      </c>
+      <c r="E5">
+        <v>0.90842865118018501</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>130</v>
+      </c>
+      <c r="B6">
+        <v>0.542185131871735</v>
+      </c>
+      <c r="C6">
+        <v>0.63930569693966999</v>
+      </c>
+      <c r="D6">
+        <v>0.64662630601860704</v>
+      </c>
+      <c r="E6">
+        <v>0.67565411551627297</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7">
+        <v>0.338884305700136</v>
+      </c>
+      <c r="C7">
+        <v>0.475385897569164</v>
+      </c>
+      <c r="D7">
+        <v>0.52131505379659304</v>
+      </c>
+      <c r="E7">
+        <v>0.54618426545592003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>132</v>
+      </c>
+      <c r="B8">
+        <v>0.46344538742345798</v>
+      </c>
+      <c r="C8">
+        <v>0.57557190558245097</v>
+      </c>
+      <c r="D8">
+        <v>0.60460040299245199</v>
+      </c>
+      <c r="E8">
+        <v>0.62727284115202497</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B9">
+        <v>0.51276177045692595</v>
+      </c>
+      <c r="C9">
+        <v>0.61692626988087296</v>
+      </c>
+      <c r="D9">
+        <v>0.62844741599200604</v>
+      </c>
+      <c r="E9">
+        <v>0.65661235587094802</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10">
+        <v>0.87178488065798998</v>
+      </c>
+      <c r="C10">
+        <v>0.99285753900806095</v>
+      </c>
+      <c r="D10">
+        <v>0.99486780567810995</v>
+      </c>
+      <c r="E10">
+        <v>0.97916563308009696</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B11">
+        <v>0.91668640504280696</v>
+      </c>
+      <c r="C11">
+        <v>0.98422385394573197</v>
+      </c>
+      <c r="D11">
+        <v>0.99189906957057805</v>
+      </c>
+      <c r="E11">
+        <v>0.96298882072934699</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>121</v>
+      </c>
+      <c r="B12">
+        <v>0.89280132864912298</v>
+      </c>
+      <c r="C12">
+        <v>0.98839561864733605</v>
+      </c>
+      <c r="D12">
+        <v>0.99332246442253702</v>
+      </c>
+      <c r="E12">
+        <v>0.97078474066578402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>127</v>
+      </c>
+      <c r="B13">
+        <v>0.86903984665870604</v>
+      </c>
+      <c r="C13">
+        <v>0.91628366470336897</v>
+      </c>
+      <c r="D13">
+        <v>0.90856541331970297</v>
+      </c>
+      <c r="E13">
+        <v>0.92143840816887901</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B14">
+        <v>0.910506426095962</v>
+      </c>
+      <c r="C14">
+        <v>0.89144927024841303</v>
+      </c>
+      <c r="D14">
+        <v>0.88854957033287396</v>
+      </c>
+      <c r="E14">
+        <v>0.89527373286810696</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B15">
+        <v>0.88882164955139098</v>
+      </c>
+      <c r="C15">
+        <v>0.90296375930309203</v>
+      </c>
+      <c r="D15">
+        <v>0.89712021341829495</v>
+      </c>
+      <c r="E15">
+        <v>0.90697302014538705</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>118</v>
+      </c>
+      <c r="C16">
+        <v>3.2297968864440897E-2</v>
+      </c>
+      <c r="D16">
+        <v>2.12887208908796E-2</v>
+      </c>
+      <c r="E16">
+        <v>0.114948533475399</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C17">
+        <v>1.9866256713867101</v>
+      </c>
+      <c r="D17">
+        <v>1.7630760669708201</v>
+      </c>
+      <c r="E17">
+        <v>1.5273951292037899</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
text_summ: finished cross validation experiment
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9430352-F9A6-4337-A875-B6A9EB79D9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BFC414-A1BB-4886-AAAB-B6A3F2EE5F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="logs-1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="143">
   <si>
     <t>Log ID</t>
   </si>
@@ -461,16 +461,37 @@
   </si>
   <si>
     <t>bart-base_lora-512-512-0_ebs-8_lr-0.0008-step-1-0.999_pt2_checkpoint-3900</t>
+  </si>
+  <si>
+    <t>kfold0</t>
+  </si>
+  <si>
+    <t>kfold1</t>
+  </si>
+  <si>
+    <t>kfold2</t>
+  </si>
+  <si>
+    <t>kfold3</t>
+  </si>
+  <si>
+    <t>kfold4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2818,7 +2839,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{7C849BBB-4DC5-45E0-BCB8-5778C27377E3}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6341,18 +6362,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
-  <dimension ref="A1:T24"/>
+  <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q20" sqref="Q20"/>
+      <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
@@ -7830,8 +7851,269 @@
         <v>6</v>
       </c>
     </row>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>138</v>
+      </c>
+      <c r="B25" s="2" t="str">
+        <f>CONCATENATE(E25,"_uf-",F25,"_ebs-",I25*K25,"_lr-",L25,"-",M25,"_",A25)</f>
+        <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_kfold0</v>
+      </c>
+      <c r="C25" s="2" t="str">
+        <f t="shared" ref="C25" si="4">CONCATENATE(E25,"_uf-",F25,"_lora-",G25,"_nepoch-",H25,"_ebs-",I25*K25,"_lr-",L25,"-",M25,"_drop-",N25,"_wd-",O25)</f>
+        <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>79</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H25">
+        <v>15</v>
+      </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>2</v>
+      </c>
+      <c r="K25">
+        <v>4</v>
+      </c>
+      <c r="L25" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N25" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O25">
+        <v>0</v>
+      </c>
+      <c r="P25" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" s="2" t="str">
+        <f>CONCATENATE(E26,"_uf-",F26,"_ebs-",I26*K26,"_lr-",L26,"-",M26,"_",A26)</f>
+        <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_kfold1</v>
+      </c>
+      <c r="C26" s="2" t="str">
+        <f t="shared" ref="C26:C29" si="5">CONCATENATE(E26,"_uf-",F26,"_lora-",G26,"_nepoch-",H26,"_ebs-",I26*K26,"_lr-",L26,"-",M26,"_drop-",N26,"_wd-",O26)</f>
+        <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>79</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26">
+        <v>15</v>
+      </c>
+      <c r="I26">
+        <v>2</v>
+      </c>
+      <c r="J26">
+        <v>2</v>
+      </c>
+      <c r="K26">
+        <v>4</v>
+      </c>
+      <c r="L26" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>140</v>
+      </c>
+      <c r="B27" s="2" t="str">
+        <f>CONCATENATE(E27,"_uf-",F27,"_ebs-",I27*K27,"_lr-",L27,"-",M27,"_",A27)</f>
+        <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_kfold2</v>
+      </c>
+      <c r="C27" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>79</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H27">
+        <v>15</v>
+      </c>
+      <c r="I27">
+        <v>2</v>
+      </c>
+      <c r="J27">
+        <v>2</v>
+      </c>
+      <c r="K27">
+        <v>4</v>
+      </c>
+      <c r="L27" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>141</v>
+      </c>
+      <c r="B28" s="2" t="str">
+        <f>CONCATENATE(E28,"_uf-",F28,"_ebs-",I28*K28,"_lr-",L28,"-",M28,"_",A28)</f>
+        <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_kfold3</v>
+      </c>
+      <c r="C28" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E28" t="s">
+        <v>2</v>
+      </c>
+      <c r="F28" t="s">
+        <v>79</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28">
+        <v>15</v>
+      </c>
+      <c r="I28">
+        <v>2</v>
+      </c>
+      <c r="J28">
+        <v>2</v>
+      </c>
+      <c r="K28">
+        <v>4</v>
+      </c>
+      <c r="L28" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O28">
+        <v>0</v>
+      </c>
+      <c r="P28" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="2" t="str">
+        <f>CONCATENATE(E29,"_uf-",F29,"_ebs-",I29*K29,"_lr-",L29,"-",M29,"_",A29)</f>
+        <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_kfold4</v>
+      </c>
+      <c r="C29" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>79</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29">
+        <v>15</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>2</v>
+      </c>
+      <c r="K29">
+        <v>4</v>
+      </c>
+      <c r="L29" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+      <c r="P29" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:T1" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
text_summ: first cut of SentenceTransformer and TSNE for visualizing dataset
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72BFC414-A1BB-4886-AAAB-B6A3F2EE5F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87238E03-54E6-421E-94DD-D92D53CD6595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="logs-1" sheetId="2" r:id="rId1"/>
@@ -556,6 +556,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Rouge</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2828,7 +2853,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1C54EF21-B404-48C9-B75B-1BFB5F9FE0C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2850,7 +2875,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8675165" cy="6296766"/>
+    <xdr:ext cx="8669461" cy="6296766"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -6364,7 +6389,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
   <dimension ref="A1:T29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
@@ -8123,7 +8148,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" activeCellId="1" sqref="A1:E1 A10:E15"/>
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
text_summ: add some regularization experiments; more investigations into the dataset
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87238E03-54E6-421E-94DD-D92D53CD6595}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B803D3B-D352-46C0-8EFA-6D159E89969A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="logs-1" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="148">
   <si>
     <t>Log ID</t>
   </si>
@@ -476,6 +476,21 @@
   </si>
   <si>
     <t>kfold4</t>
+  </si>
+  <si>
+    <t>Unfreeze LM head</t>
+  </si>
+  <si>
+    <t>lm-head</t>
+  </si>
+  <si>
+    <t>Unfreeze LM head, apply dropout</t>
+  </si>
+  <si>
+    <t>Unfreeze LM head, apply weight decay</t>
+  </si>
+  <si>
+    <t>0.2-0.2-0.2</t>
   </si>
 </sst>
 </file>
@@ -2853,7 +2868,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{1C54EF21-B404-48C9-B75B-1BFB5F9FE0C7}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="167" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="167" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3257,8 +3272,8 @@
   <dimension ref="A1:Q102"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A37" sqref="A37:XFD37"/>
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6387,17 +6402,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
-  <dimension ref="A1:T29"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="66.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.140625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
@@ -7937,7 +7952,7 @@
         <v>bart-base_uf-all_ebs-8_lr-0.0004-step-1-0.998_kfold1</v>
       </c>
       <c r="C26" s="2" t="str">
-        <f t="shared" ref="C26:C29" si="5">CONCATENATE(E26,"_uf-",F26,"_lora-",G26,"_nepoch-",H26,"_ebs-",I26*K26,"_lr-",L26,"-",M26,"_drop-",N26,"_wd-",O26)</f>
+        <f t="shared" ref="C26:C30" si="5">CONCATENATE(E26,"_uf-",F26,"_lora-",G26,"_nepoch-",H26,"_ebs-",I26*K26,"_lr-",L26,"-",M26,"_drop-",N26,"_wd-",O26)</f>
         <v>bart-base_uf-all_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
       </c>
       <c r="D26" s="2" t="s">
@@ -8133,6 +8148,214 @@
         <v>0</v>
       </c>
       <c r="P29" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>143</v>
+      </c>
+      <c r="B30" s="2" t="str">
+        <f t="shared" ref="B30" si="6">CONCATENATE(E30,"_uf-",F30,"_ebs-",I30*K30,"_lr-",L30,"-",M30)</f>
+        <v>bart-base_uf-lm-head_ebs-8_lr-0.0004-step-1-0.998</v>
+      </c>
+      <c r="C30" s="2" t="str">
+        <f t="shared" si="5"/>
+        <v>bart-base_uf-lm-head_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-0</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H30">
+        <v>15</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>2</v>
+      </c>
+      <c r="K30">
+        <v>4</v>
+      </c>
+      <c r="L30" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+      <c r="P30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>145</v>
+      </c>
+      <c r="B31" s="2" t="str">
+        <f>CONCATENATE(E31,"_uf-",F31,"_ebs-",I31*K31,"_lr-",L31,"-",M31,"_drop-",N31)</f>
+        <v>bart-base_uf-lm-head_ebs-8_lr-0.0004-step-1-0.998_drop-0.2-0.2-0.2</v>
+      </c>
+      <c r="C31" s="2" t="str">
+        <f t="shared" ref="C31" si="7">CONCATENATE(E31,"_uf-",F31,"_lora-",G31,"_nepoch-",H31,"_ebs-",I31*K31,"_lr-",L31,"-",M31,"_drop-",N31,"_wd-",O31)</f>
+        <v>bart-base_uf-lm-head_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.2-0.2-0.2_wd-0</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>144</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H31">
+        <v>15</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>2</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+      <c r="L31" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O31">
+        <v>0</v>
+      </c>
+      <c r="P31" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="2" t="str">
+        <f>CONCATENATE(E32,"_uf-",F32,"_ebs-",I32*K32,"_lr-",L32,"-",M32,"_drop-",N32,"_pt2")</f>
+        <v>bart-base_uf-lm-head_ebs-8_lr-0.0004-step-1-0.998_drop-0.2-0.2-0.2_pt2</v>
+      </c>
+      <c r="C32" s="2" t="str">
+        <f t="shared" ref="C32:C33" si="8">CONCATENATE(E32,"_uf-",F32,"_lora-",G32,"_nepoch-",H32,"_ebs-",I32*K32,"_lr-",L32,"-",M32,"_drop-",N32,"_wd-",O32)</f>
+        <v>bart-base_uf-lm-head_lora-none_nepoch-30_ebs-8_lr-0.0004-step-1-0.998_drop-0.2-0.2-0.2_wd-0</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>144</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H32">
+        <v>30</v>
+      </c>
+      <c r="I32">
+        <v>2</v>
+      </c>
+      <c r="J32">
+        <v>2</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
+      <c r="L32" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N32" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="O32">
+        <v>0</v>
+      </c>
+      <c r="P32" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>146</v>
+      </c>
+      <c r="B33" s="2" t="str">
+        <f>CONCATENATE(E33,"_uf-",F33,"_ebs-",I33*K33,"_lr-",L33,"-",M33,"_wd-",O33)</f>
+        <v>bart-base_uf-lm-head_ebs-8_lr-0.0004-step-1-0.998_wd-4</v>
+      </c>
+      <c r="C33" s="2" t="str">
+        <f t="shared" si="8"/>
+        <v>bart-base_uf-lm-head_lora-none_nepoch-15_ebs-8_lr-0.0004-step-1-0.998_drop-0.1-0.1-0.1_wd-4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>144</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H33">
+        <v>15</v>
+      </c>
+      <c r="I33">
+        <v>2</v>
+      </c>
+      <c r="J33">
+        <v>2</v>
+      </c>
+      <c r="K33">
+        <v>4</v>
+      </c>
+      <c r="L33" s="1">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="O33">
+        <v>4</v>
+      </c>
+      <c r="P33" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
text_summ: sanity-checked validation sample ID 209 against the rest of the dataset
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E17A8D0-2F81-47BD-B692-B723CD054838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB9E6A-A887-43C6-8B91-660023DBE50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="20985" activeTab="2" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="6" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
   <sheets>
     <sheet name="logs-1-old-format" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,13 @@
     <sheet name="rouge" sheetId="9" r:id="rId4"/>
     <sheet name="bertscore" sheetId="10" r:id="rId5"/>
     <sheet name="predictions" sheetId="4" r:id="rId6"/>
+    <sheet name="text analysis" sheetId="12" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">logs!$A$1:$U$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'logs-1'!$A$1:$R$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'logs-1-old-format'!$A$1:$AI$102</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'text analysis'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1470" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="305">
   <si>
     <t>Log ID</t>
   </si>
@@ -724,6 +726,343 @@
   </si>
   <si>
     <t>**Unfreeze lm-head, sweep weight decay, linear LR</t>
+  </si>
+  <si>
+    <t>Split</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Dialogue</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Reference sample</t>
+  </si>
+  <si>
+    <t>Val</t>
+  </si>
+  <si>
+    <t>Symptoms: refracture of right forearm
+Diagnosis: complete fractures of both bones in right arm, shortening bayonet apposition
+History of Patient: fell onto right arm on December 5, 2007
+Plan of Action: surgery for closed reduction and pinning, with risks including anesthesia, infection, bleeding, changes in sensation and motion of extremity, hardware failure, need for later hardware removal, cast tightness</t>
+  </si>
+  <si>
+    <t>Train</t>
+  </si>
+  <si>
+    <t>Dialogue similarity ranking</t>
+  </si>
+  <si>
+    <t>Summary similarity ranking</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Noise</t>
+  </si>
+  <si>
+    <t>&gt; 10</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>When was the last time you got a tetanus shot?</t>
+  </si>
+  <si>
+    <t>Patient with history of falling does not want chair and bed monitor</t>
+  </si>
+  <si>
+    <t>Patient has history of osteomyelitis in right fifth toe and diabetes mellitus</t>
+  </si>
+  <si>
+    <t>Patient fell onto right hip and lower back while bringing in groceries from car</t>
+  </si>
+  <si>
+    <t>t-SNE perplexity = 10</t>
+  </si>
+  <si>
+    <t>Fracture</t>
+  </si>
+  <si>
+    <t>Two doctors talking about patient history - surgeries and right hip fracture</t>
+  </si>
+  <si>
+    <t>Patient hurt back of left thigh; patient hurt kneecap while boat fishing and got surgery; patient has external fixation on knee while the fracture heals</t>
+  </si>
+  <si>
+    <t>Patient fell onto right arm and completely fractured both arm bones; doctor suggests surgery and says that risk of infection is less than one percent with antibiotics; other surgical risks include bleeding, etc.</t>
+  </si>
+  <si>
+    <t>Patient fractured left elbow and underwent ORIF surgery; doctor says fracture has healed well; patient has been going to physical therapy; doctor says another surgery is required to remove hardware and says that risk of infection is less than one percent with antibiotics; other surgical risks include bleeding, etc.</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: 10-year-old right-hand dominant male threw himself off a quad on 10/10/2007, underwent open reduction and internal fixation of left elbow fracture dislocation, sustained nondisplaced right glenoid neck fracture, experiencing postoperative stiffness treated with physical therapy and Dynasplint, neurologically intact distally
+Plan of Action: Surgery recommended for hardware removal from left elbow to decrease irritation with elbow extension, risks discussed include anesthesia, infection, bleeding, changes in sensation and motion of extremities, failure to remove hardware, failure to relieve pain, continued postoperative stiffness; parents agreed to the plan</t>
+  </si>
+  <si>
+    <t>Patient came in for surgery to fix acute on chronic right slipped capital femoral epiphysis; X-ray shows screw is going into the hip joint; doctor says another operation is required to remove the screw and replace it with a shorter one; doctor says risk of infection is less than one percent; other surgical risks include bleeding, etc.</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: acute on chronic right slipped capital femoral epiphysis
+History of Patient: presented in November
+Plan of Action: underwent in situ pinning, screw exchange discussed</t>
+  </si>
+  <si>
+    <t>Patient jumped off swing and suffered a closed type three supracondylar fracture of left distal humerus</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: patient had cardioversion for atrial fibrillation, taking Coumadin, history of smoking but quit several years ago, denies COPD or emphysema, no family members are sick
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Doctor says X-ray does not show any open fracture or bone abnormality</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: N/A
+Plan of Action: N/A
+.</t>
+  </si>
+  <si>
+    <t>Doctor asks patient when the surgery happened</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: slipped capital femoral epiphysis (SCFE) bilaterally
+History of Patient: post-surgery, 2-1/2 months
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient hit left elbow against a railing trying to do a new trick on skateboard; patient has iced the elbow, but the pain has only gotten worse; patient has not taken Advil or Tylenol</t>
+  </si>
+  <si>
+    <t>Symptoms: Left elbow pain.
+Diagnosis: N/A.
+History of Patient: Injured left elbow by hitting it against a railing while attempting a new trick on a skateboard about a week ago, pain came on gradually, no other body parts injured, hasn't taken any medication for the pain.
+Plan Of Action: N/A.</t>
+  </si>
+  <si>
+    <t>Patient injured elbow during a fight in juvenile hall; patient has left ankle pain; patient hit head against the floor during fight but does not have headache, nausea, blurry vision, or chest or abdominal pain</t>
+  </si>
+  <si>
+    <t>Symptoms: Pain in the left elbow and left ankle.
+Diagnosis: N/A
+History of Patient: The 17-year-old male sustained an elbow injury during a fight with other kids in Juvenile Hall, experiencing sudden pain in his left elbow. He also reports pain in his left ankle, with previous left knee pain. He denies passing out, neck pain, chest pain, or abdominal pain. No weapons were involved in the fight.
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Symptoms: Pain in left elbow and left ankle, previous pain in left knee
+Diagnosis: N/A
+History of Complaint: 17-year-old male experienced pain in left elbow and left ankle during a fight in Juvenile Hall, denies neck pain despite being hit in the head, no chest or abdominal pain, no weapons involved
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient injured left elbow during fight in juvie; patient has left ankle pain; patient got hit in the head; patient does not have chest or abdominal pain</t>
+  </si>
+  <si>
+    <t>Patient splashed hot oil onto his arm while working in coffee shop kitchen and was burned from elbow to wrist</t>
+  </si>
+  <si>
+    <t>Symptoms: Burn on the arm from elbow to wrist, mainly on the medial aspect
+Diagnosis: N/A
+History of Complaint: Workers' Compensation injury, hot oil splashed onto arm while cooking in coffee shop kitchen
+Plan of Action: Provide care for burn injury</t>
+  </si>
+  <si>
+    <t>Patient underwent screw compression to fix distracted left lateral condyle fracture; patient is coming in to remove the hardware; doctor says surgical risks include anesthesia, infection, bleeding, etc.</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: distracted left lateral condyle fracture
+History of Patient: Underwent screw compression for the fracture in October 2007, now presents for hardware removal
+Plan of Action: Risks and benefits of surgery discussed, including risk of anesthesia, infection, bleeding, changes in sensation and motion of extremity, failure of removal of hardware, failure to relieve pain or improve range of motion; family agreed to the plan</t>
+  </si>
+  <si>
+    <t>Doctor looks at patient's ultrasound</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A.
+Diagnosis: N/A.
+History of Patient: N/A.
+Plan of Action: The only significant finding in the ultrasound of the area is that it shows this to be related to bone.</t>
+  </si>
+  <si>
+    <t>Patient twisted right ankle while running</t>
+  </si>
+  <si>
+    <t>Symptoms: right ankle pain on the lateral aspect
+Diagnosis: N/A
+History of Patient: twisted right ankle while running, no other injuries, brought in by mother, primary care physician is Dr. Brown
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient plays basketball for University of Houston; patient landed on another player's foot, was taped up, and kept playing; patient's foot is swollen and can't put weight on it; patient is in a walking boot</t>
+  </si>
+  <si>
+    <t>Symptoms: Swelling, pain onset immediately after injury, pain with weightbearing activities, limping
+Diagnosis: Inversion injury, tenderness around the navicular
+History of Patient: Injured foot during basketball game while traveling to Duke, landed on another player's foot, taped by trainer John Houston, continued playing after injury
+Plan of Action: Patient has been in a walking boot, foot taped firmly, advised to continue wearing the tape, continue monitoring for pain and swelling</t>
+  </si>
+  <si>
+    <t>Following ORIF surgery to fix right tibial plateau fracture, patient had surgery one week ago to remove Ex Fix from the right knee with MUA to break up scar tissue; patient does not have much pain, flu symptoms, numbness, or tingling; patient is doing range of motion exercises</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: Approximately one week status post removal of Ex-Fix from the right knee with manipulation under anesthesia (MUA) following open reduction internal fixation (ORIF) of right tibial plateau fracture, well-controlled pain, mild drainage from pin sites, just started range of motion exercises for the right knee, no fevers, chills, or night sweats, no numbness or tingling
+Plan of Action: Continue range of motion exercises, monitor pin sites for drainage, follow-up as scheduled</t>
+  </si>
+  <si>
+    <t>Patient has a right side shoulder strain and possibly some nerve compression</t>
+  </si>
+  <si>
+    <t>Symptoms: Right shoulder pain, most likely secondary to muscular strain
+Diagnosis: very mild evidence of impingement
+History of Patient: N/A
+Plan of Action: Further evaluation and treatment will be done.</t>
+  </si>
+  <si>
+    <t>Patient had knee replacement surgery for both knees three years ago and is now having pain in both knees</t>
+  </si>
+  <si>
+    <t>Symptoms: pain in both knees
+Diagnosis: N/A
+History of Patient: bilateral knee replacement three years ago, experiencing pain in both knees
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient injured left knee after slipping in a grocery store; patient's primary care provider gave him a knee brace and referred him to physical therapy</t>
+  </si>
+  <si>
+    <t>Symptoms: left knee pain
+Diagnosis: N/A
+History of Patient: fell in grocery store on 10/02/08, slipped on grape, went to ED then followed up with PCP, referred to Physical Therapy, received knee brace
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Two doctors talking about patient - multiple areas with hypergranulation tissue on the left leg</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: N/A
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient underwent percutaneous screw fixation of a Schatzker I V tibial plateau fracture; patient has been going to physical therapy; patient says there are no signs of infection; patient has no fever symptoms but has some tingling in feet</t>
+  </si>
+  <si>
+    <t>Symptoms: Tingling in both feet.
+Diagnosis: N/A.
+History of Patient: 59-year-old male, 4 months post percutaneous screw fixation of Schatzker IV tibial plateau fracture and nonoperative management of second through fifth metatarsal head fractures. Currently at home after leaving nursing home facility. Pain well controlled. Working with physical therapy 2-3 times a week. No drainage or fever. History of spinal stenosis with lower extremity neuropathy.
+Plan of Action: N/A.</t>
+  </si>
+  <si>
+    <t>Patient had circumcision and had minor post-op bleeding</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: phimosis (resolved)
+History of Patient: circumcision performed on 09/16/2007 at Children's Hospital, minor bleeding post-operation requiring additional sutures, pain managed with oral analgesics for a couple of days, normal urination and bowel movements
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient has pain in navicular bone, and wearing shoes makes it worse; patient has had surgery for osteochondroma in the foot; patient requests surgery</t>
+  </si>
+  <si>
+    <t>Symptoms: extreme pain over the navicular bone with shoe gear.
+Diagnosis: hereditary osteochondromas, previous dissection of osteochondromas.
+History of Patient: pain in the foot, multiple osteochondromas of unknown origin, desire for surgical treatment.
+Plan of Action: surgical treatment for pain in the foot caused by osteochondromas.</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A.
+Diagnosis: N/A.
+History of Patient: N/A.
+Plan of Action: N/A.</t>
+  </si>
+  <si>
+    <t>Patient has stomach pain</t>
+  </si>
+  <si>
+    <t>Symptoms: pain in my tummy.
+Diagnosis: left patellar chondromalacia.
+History of Patient: started suddenly around noon.
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A.
+Diagnosis: N/A.
+History of Patient: History of multiple falls.
+Plan of Action: Recommending chair and bed monitor for fall detection, patient declined.</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: Diabetes mellitus, history of osteomyelitis of the right fifth toe treated with IV antibiotics therapy 5 years ago for 6 weeks
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Symptoms: back pain
+Diagnosis: N/A
+History of Patient: fell on steps three nights ago while bringing in groceries, landed on right hip and hit low back on railing
+Plan of Action: doctor wants to get imaging done</t>
+  </si>
+  <si>
+    <t>Patient recounts past surgeries: craniotomy for brain hemorrhage, leg surgery to fix fracture, stomach surgery as a child</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: 1. Surgery on stomach as a child. Type unknown, common procedure with no complications. 2. Surgery for leg fracture with pins inserted. 3. Craniotomy seven years ago for intracranial hemorrhage/subdural hematoma.
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Patient is undergoing conservative treatment for lower back fracture, but there's been no improvement; doctor recommends bileral L five kyphoplasty to fix incomplete healing of L five compression fracture; doctor says risk of infection is less than one percent with antibiotics</t>
+  </si>
+  <si>
+    <t>Symptoms: back and buttock pain
+Diagnosis: L5 compression fracture with sclerosis, incomplete healing
+History of Patient: 86-year-old female with history of back and buttock pain, conservative treatment unsuccessful, CT scan shows incomplete healing of L5 compression fracture
+Plan of Action: bilateral L5 kyphoplasty scheduled, patient denies bowel or bladder incontinence, wears back brace and corset, no weakness reported</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A.
+Diagnosis: N/A.
+History of Patient: Appendectomy, right hip fracture from a fall in 2005, total abdominal hysterectomy (TAH) with bilateral salpingo-oophorectomy (BSO).
+Plan of Action: N/A.</t>
+  </si>
+  <si>
+    <t>Symptoms: pain and injury to the back of left thigh, knee injury from a boat accident, hypergranulation tissue around graft site, drainage from areas with hypergranulation tissue.
+Diagnosis: N/A.
+History of Patient: traumatic injury to left posterior thigh, surgery for large defect in left posterior thigh, ongoing external fixation for healing fractures in leg, grafting and full thickness skin grafting for closure of defect, nearly healed in gluteal fold area.
+Plan of Action: referred to clinic for management of hypergranulation tissue and drainage from graft site.</t>
+  </si>
+  <si>
+    <t>Patient fell off liner ten feet and landed on left foot; no deformity in ankle but X-ray shows fractured talus (heel); doctor recommends surgery to repair ankle; risk of infection is low</t>
+  </si>
+  <si>
+    <t>Symptoms: left ankle pain, disfigurement
+Diagnosis: grade IV Hawkins fracture of left talus
+History of Patient: 50-year-old male, fell from approximately 10 feet onto left foot, no other injuries reported, distal neurovascularly intact
+Plan of Action: surgery recommended due to risk of avascular necrosis, risks of infection discussed and antibiotics planned</t>
+  </si>
+  <si>
+    <t>Rouge</t>
   </si>
 </sst>
 </file>
@@ -765,12 +1104,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -12246,9 +12594,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A33" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14511,4 +14859,781 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680AF2A0-B839-4572-9E69-3A99B736CEC3}">
+  <dimension ref="A1:M49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" style="4" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="4"/>
+    <col min="4" max="4" width="78.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="130" style="4" customWidth="1"/>
+    <col min="6" max="7" width="11.7109375" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>304</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C2" s="5">
+        <v>209</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="B3" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C3" s="5">
+        <v>727</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="F3" s="6">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C4" s="6">
+        <v>649</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>266</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="F4" s="6">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C5" s="6">
+        <v>902</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1097</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>298</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B7" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C7" s="5">
+        <v>182</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="F7" s="6">
+        <v>2</v>
+      </c>
+      <c r="G7" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C8" s="6">
+        <v>640</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>275</v>
+      </c>
+      <c r="F8" s="6">
+        <v>5</v>
+      </c>
+      <c r="G8" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C9" s="6">
+        <v>606</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>285</v>
+      </c>
+      <c r="F9" s="6">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C10" s="6">
+        <v>931</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="F10" s="6">
+        <v>3</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C11" s="6">
+        <v>219</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11" s="6">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C12" s="6">
+        <v>194</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="F12" s="6">
+        <v>5</v>
+      </c>
+      <c r="G12" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C13" s="6">
+        <v>401</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G13" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="B14" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C14" s="6">
+        <v>1155</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G14" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="B15" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1290</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G15" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="B16" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C16" s="6">
+        <v>1240</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>264</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>265</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G16" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B17" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1160</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>268</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>269</v>
+      </c>
+      <c r="F17" s="6">
+        <v>2</v>
+      </c>
+      <c r="G17" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B18" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C18" s="6">
+        <v>616</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>270</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="F18" s="6">
+        <v>3</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B19" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" s="6">
+        <v>1009</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="F19" s="6">
+        <v>4</v>
+      </c>
+      <c r="G19" s="6">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B20" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C20" s="6">
+        <v>1181</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>276</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G20" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B21" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C21" s="6">
+        <v>273</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>278</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>279</v>
+      </c>
+      <c r="F21" s="6">
+        <v>10</v>
+      </c>
+      <c r="G21" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" s="6">
+        <v>877</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>281</v>
+      </c>
+      <c r="F22" s="6">
+        <v>7</v>
+      </c>
+      <c r="G22" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C23" s="6">
+        <v>540</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="F23" s="6">
+        <v>1</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B24" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C24" s="6">
+        <v>257</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>286</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="F24" s="6">
+        <v>3</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B25" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C25" s="6">
+        <v>521</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>288</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="F25" s="6">
+        <v>4</v>
+      </c>
+      <c r="G25" s="6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B26" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" s="6">
+        <v>89</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="F26" s="6">
+        <v>5</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" s="6">
+        <v>308</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>292</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G27" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B28" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C28" s="6">
+        <v>88</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G28" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B29" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C29" s="6">
+        <v>678</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="F29" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="G29" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="B30" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="C30" s="6">
+        <v>367</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="F30" s="6">
+        <v>6</v>
+      </c>
+      <c r="G30" s="6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C31" s="6">
+        <v>814</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C32" s="6">
+        <v>398</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>300</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C33" s="6">
+        <v>514</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+    </row>
+    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+    </row>
+    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+    </row>
+    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+    </row>
+    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+    </row>
+    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+    </row>
+    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="C48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+    </row>
+    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1" xr:uid="{680AF2A0-B839-4572-9E69-3A99B736CEC3}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
text_summ: finished first draft of report
</commit_message>
<xml_diff>
--- a/text_summ/experiment_tracker.xlsx
+++ b/text_summ/experiment_tracker.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ml_ai_portfolio\text_summ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BBB9E6A-A887-43C6-8B91-660023DBE50C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2B6340-9D66-47CD-B19C-DEDAF62AA741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" firstSheet="1" activeTab="6" xr2:uid="{0AC54277-F8AF-4AEE-83BD-EC3E26374A59}"/>
   </bookViews>
@@ -25,7 +25,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">logs!$A$1:$U$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'logs-1'!$A$1:$R$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'logs-1-old-format'!$A$1:$AI$102</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'text analysis'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'text analysis'!$A$1:$H$33</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1604" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1618" uniqueCount="315">
   <si>
     <t>Log ID</t>
   </si>
@@ -1062,7 +1062,48 @@
 Plan of Action: surgery recommended due to risk of avascular necrosis, risks of infection discussed and antibiotics planned</t>
   </si>
   <si>
-    <t>Rouge</t>
+    <t>Loss</t>
+  </si>
+  <si>
+    <t>Bertscore (F1)</t>
+  </si>
+  <si>
+    <t>Rouge1</t>
+  </si>
+  <si>
+    <t>Rouge2</t>
+  </si>
+  <si>
+    <t>RougeL</t>
+  </si>
+  <si>
+    <t>RougeLsum</t>
+  </si>
+  <si>
+    <t>Prediction</t>
+  </si>
+  <si>
+    <t>Symptoms: fell onto right arm on December 5, 2007, incomplete fractures of both bones in right arm, shortening bayonet apposition, possible need for later hardware removal and possible continuous nerve Symptoms
+Diagnosis: N/A
+History of Patient: fell onto right arm on December 5, 2007, incomplete fractures of both bones, received physical therapy and bandaging, no other surgeries recommended due to risk of infection
+Plan of Action: Surgery recommended due to non-healing extremity injuries, risks of infection discussed and patient agreed to surgery after informed consent</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: N/A
+History of Patient: distracted left lateral condyle fracture (PUD) with screw compression to prevent fracture
+Plan of Action: N/A</t>
+  </si>
+  <si>
+    <t>Symptoms: N/A
+Diagnosis: right tibial plateau fracture
+History of Patient: surgery performed approximately a week ago for right tibial plateau fracture, previous surgery for right tibial plateau fracture, unsuccessful interventional management strategies</t>
+  </si>
+  <si>
+    <t>Symptoms: percutaneous screw fixation of a Schatzker I V tibial plateau fracture, toe fractures nonoperatively, no pain, no injuries reported, has a history of spinal stenosis, severe cough, runny nose, sore throat, fatigue, and tingling in both feet.
+Diagnosis: percutaneous screw fixation of a Schatzker I V tibial plateau fracture, toe fractures nonoperatively, no other associated injuries.
+History of Patient: toe fractures and tingling in both feet, history of spinal stenosis, and neuropathy, post-surgery, normal side effects, no prior history of spinal stenosis, and neuropathy.
+Plan of Action: N/A</t>
   </si>
 </sst>
 </file>
@@ -1104,7 +1145,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -1119,6 +1160,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1800,6 +1844,31 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>BERTScore</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3504,7 +3573,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8675165" cy="6296766"/>
+    <xdr:ext cx="8669461" cy="6296766"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -12594,9 +12663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26AAD59C-1F2A-44F2-B5D4-832F7DFE9B93}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+      <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14561,7 +14630,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14863,23 +14932,32 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{680AF2A0-B839-4572-9E69-3A99B736CEC3}">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.7109375" style="4" customWidth="1"/>
-    <col min="2" max="3" width="9.140625" style="4"/>
-    <col min="4" max="4" width="78.140625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="130" style="4" customWidth="1"/>
-    <col min="6" max="7" width="11.7109375" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="1" max="1" width="10.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="7.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="117.5703125" style="4" customWidth="1"/>
+    <col min="6" max="6" width="111.28515625" style="4" customWidth="1"/>
+    <col min="7" max="8" width="11.7109375" style="4" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="4" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" style="4" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="4" customWidth="1"/>
+    <col min="14" max="14" width="11" style="4" customWidth="1"/>
+    <col min="15" max="15" width="11.5703125" style="4" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>27</v>
       </c>
@@ -14896,19 +14974,37 @@
         <v>228</v>
       </c>
       <c r="F1" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>234</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>304</v>
       </c>
+      <c r="J1" s="4" t="s">
+        <v>305</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>306</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>307</v>
+      </c>
       <c r="M1" s="4" t="s">
+        <v>308</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>309</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>229</v>
       </c>
@@ -14924,14 +15020,35 @@
       <c r="E2" s="4" t="s">
         <v>231</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>235</v>
+      <c r="F2" s="4" t="s">
+        <v>311</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+      <c r="H2" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="7">
+        <v>1.7847547531127901</v>
+      </c>
+      <c r="J2" s="7">
+        <v>0.88533043861389105</v>
+      </c>
+      <c r="K2" s="7">
+        <v>0.54794520547945202</v>
+      </c>
+      <c r="L2" s="7">
+        <v>0.36111111111111099</v>
+      </c>
+      <c r="M2" s="7">
+        <v>0.41095890410958902</v>
+      </c>
+      <c r="N2" s="7">
+        <v>0.52054794520547898</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="120" hidden="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
         <v>232</v>
       </c>
@@ -14944,14 +15061,35 @@
       <c r="E3" s="4" t="s">
         <v>249</v>
       </c>
-      <c r="F3" s="6">
-        <v>1</v>
+      <c r="F3" s="4" t="s">
+        <v>249</v>
       </c>
       <c r="G3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1.7603058367967599E-2</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <v>1</v>
+      </c>
+      <c r="N3" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
         <v>230</v>
       </c>
@@ -14964,14 +15102,35 @@
       <c r="E4" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="F4" s="6">
-        <v>1</v>
+      <c r="F4" s="4" t="s">
+        <v>312</v>
       </c>
       <c r="G4" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="7">
+        <v>1.8884578943252499</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0.85258644819259599</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0.40860215053763399</v>
+      </c>
+      <c r="L4" s="7">
+        <v>0.26373626373626302</v>
+      </c>
+      <c r="M4" s="7">
+        <v>0.32258064516128998</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0.40860215053763399</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B5" s="4" t="s">
         <v>232</v>
       </c>
@@ -14984,14 +15143,35 @@
       <c r="E5" s="4" t="s">
         <v>303</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>244</v>
+      <c r="F5" s="4" t="s">
+        <v>303</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="6" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="H5" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="I5" s="7">
+        <v>4.4116326607763698E-3</v>
+      </c>
+      <c r="J5" s="7">
+        <v>1</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1</v>
+      </c>
+      <c r="L5" s="7">
+        <v>1</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>232</v>
       </c>
@@ -15004,14 +15184,35 @@
       <c r="E6" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>244</v>
+      <c r="F6" s="4" t="s">
+        <v>299</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="H6" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="I6" s="7">
+        <v>5.3094853647053198E-3</v>
+      </c>
+      <c r="J6" s="7">
+        <v>1</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1</v>
+      </c>
+      <c r="L6" s="7">
+        <v>1</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>232</v>
       </c>
@@ -15024,14 +15225,35 @@
       <c r="E7" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="F7" s="6">
-        <v>2</v>
+      <c r="F7" s="4" t="s">
+        <v>251</v>
       </c>
       <c r="G7" s="6">
+        <v>2</v>
+      </c>
+      <c r="H7" s="6">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="I7" s="7">
+        <v>4.3251626193523398E-3</v>
+      </c>
+      <c r="J7" s="7">
+        <v>1</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>230</v>
       </c>
@@ -15044,14 +15266,35 @@
       <c r="E8" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="F8" s="6">
-        <v>5</v>
+      <c r="F8" s="4" t="s">
+        <v>313</v>
       </c>
       <c r="G8" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+      <c r="H8" s="6">
+        <v>5</v>
+      </c>
+      <c r="I8" s="7">
+        <v>2.8929758071899401</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0.83574652671813898</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0.31034482758620602</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0.140350877192982</v>
+      </c>
+      <c r="M8" s="7">
+        <v>0.25862068965517199</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0.29310344827586199</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="105" hidden="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>238</v>
       </c>
@@ -15064,14 +15307,35 @@
       <c r="E9" s="4" t="s">
         <v>285</v>
       </c>
-      <c r="F9" s="6">
-        <v>2</v>
+      <c r="F9" s="4" t="s">
+        <v>314</v>
       </c>
       <c r="G9" s="6">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="H9" s="6">
+        <v>2</v>
+      </c>
+      <c r="I9" s="7">
+        <v>2.9159190654754599</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0.82634067535400302</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0.42424242424242398</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0.245398773006134</v>
+      </c>
+      <c r="M9" s="7">
+        <v>0.32727272727272699</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>236</v>
       </c>
@@ -15087,14 +15351,14 @@
       <c r="E10" s="4" t="s">
         <v>253</v>
       </c>
-      <c r="F10" s="6">
+      <c r="G10" s="6">
         <v>3</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="H10" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="B11" s="4" t="s">
         <v>232</v>
       </c>
@@ -15107,14 +15371,14 @@
       <c r="E11" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="F11" s="6">
-        <v>4</v>
-      </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="6">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
         <v>232</v>
       </c>
@@ -15127,14 +15391,14 @@
       <c r="E12" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="F12" s="6">
+      <c r="G12" s="6">
         <v>5</v>
       </c>
-      <c r="G12" s="6">
+      <c r="H12" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="B13" s="4" t="s">
         <v>232</v>
       </c>
@@ -15147,14 +15411,14 @@
       <c r="E13" s="4" t="s">
         <v>259</v>
       </c>
-      <c r="F13" s="6" t="s">
+      <c r="G13" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G13" s="6">
+      <c r="H13" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="90" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" ht="90" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
         <v>232</v>
       </c>
@@ -15167,14 +15431,14 @@
       <c r="E14" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="F14" s="6" t="s">
+      <c r="G14" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G14" s="6">
+      <c r="H14" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" ht="75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
         <v>232</v>
       </c>
@@ -15187,14 +15451,14 @@
       <c r="E15" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="G15" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G15" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="60" x14ac:dyDescent="0.25">
+      <c r="H15" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="60" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
         <v>232</v>
       </c>
@@ -15207,14 +15471,14 @@
       <c r="E16" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="F16" s="6" t="s">
+      <c r="G16" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G16" s="6">
+      <c r="H16" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>230</v>
       </c>
@@ -15227,14 +15491,14 @@
       <c r="E17" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="F17" s="6">
-        <v>2</v>
-      </c>
       <c r="G17" s="6">
+        <v>2</v>
+      </c>
+      <c r="H17" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
         <v>230</v>
       </c>
@@ -15247,14 +15511,14 @@
       <c r="E18" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="F18" s="6">
+      <c r="G18" s="6">
         <v>3</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="H18" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B19" s="4" t="s">
         <v>230</v>
       </c>
@@ -15267,14 +15531,14 @@
       <c r="E19" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="F19" s="6">
-        <v>4</v>
-      </c>
       <c r="G19" s="6">
+        <v>4</v>
+      </c>
+      <c r="H19" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>230</v>
       </c>
@@ -15287,14 +15551,14 @@
       <c r="E20" s="4" t="s">
         <v>277</v>
       </c>
-      <c r="F20" s="6" t="s">
+      <c r="G20" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G20" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H20" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>230</v>
       </c>
@@ -15307,14 +15571,14 @@
       <c r="E21" s="4" t="s">
         <v>279</v>
       </c>
-      <c r="F21" s="6">
+      <c r="G21" s="6">
         <v>10</v>
       </c>
-      <c r="G21" s="6">
+      <c r="H21" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>230</v>
       </c>
@@ -15327,14 +15591,14 @@
       <c r="E22" s="4" t="s">
         <v>281</v>
       </c>
-      <c r="F22" s="6">
+      <c r="G22" s="6">
         <v>7</v>
       </c>
-      <c r="G22" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H22" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>238</v>
       </c>
@@ -15347,14 +15611,14 @@
       <c r="E23" s="4" t="s">
         <v>283</v>
       </c>
-      <c r="F23" s="6">
+      <c r="G23" s="6">
         <v>1</v>
       </c>
-      <c r="G23" s="6" t="s">
+      <c r="H23" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
         <v>238</v>
       </c>
@@ -15367,14 +15631,14 @@
       <c r="E24" s="4" t="s">
         <v>287</v>
       </c>
-      <c r="F24" s="6">
+      <c r="G24" s="6">
         <v>3</v>
       </c>
-      <c r="G24" s="6" t="s">
+      <c r="H24" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B25" s="4" t="s">
         <v>238</v>
       </c>
@@ -15387,14 +15651,14 @@
       <c r="E25" s="4" t="s">
         <v>289</v>
       </c>
-      <c r="F25" s="6">
-        <v>4</v>
-      </c>
       <c r="G25" s="6">
+        <v>4</v>
+      </c>
+      <c r="H25" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B26" s="4" t="s">
         <v>238</v>
       </c>
@@ -15407,14 +15671,14 @@
       <c r="E26" s="4" t="s">
         <v>290</v>
       </c>
-      <c r="F26" s="6">
+      <c r="G26" s="6">
         <v>5</v>
       </c>
-      <c r="G26" s="6" t="s">
+      <c r="H26" s="6" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
         <v>236</v>
       </c>
@@ -15430,14 +15694,14 @@
       <c r="E27" s="4" t="s">
         <v>292</v>
       </c>
-      <c r="F27" s="6" t="s">
+      <c r="G27" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G27" s="6">
+      <c r="H27" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>238</v>
       </c>
@@ -15450,14 +15714,14 @@
       <c r="E28" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="F28" s="6" t="s">
+      <c r="G28" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G28" s="6">
+      <c r="H28" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B29" s="4" t="s">
         <v>238</v>
       </c>
@@ -15470,14 +15734,14 @@
       <c r="E29" s="4" t="s">
         <v>294</v>
       </c>
-      <c r="F29" s="6" t="s">
+      <c r="G29" s="6" t="s">
         <v>237</v>
       </c>
-      <c r="G29" s="6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="H29" s="6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="B30" s="4" t="s">
         <v>238</v>
       </c>
@@ -15490,14 +15754,14 @@
       <c r="E30" s="4" t="s">
         <v>295</v>
       </c>
-      <c r="F30" s="6">
+      <c r="G30" s="6">
         <v>6</v>
       </c>
-      <c r="G30" s="6">
+      <c r="H30" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B31" s="4" t="s">
         <v>232</v>
       </c>
@@ -15510,14 +15774,14 @@
       <c r="E31" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="F31" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="G31" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="H31" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
         <v>232</v>
       </c>
@@ -15530,14 +15794,14 @@
       <c r="E32" s="4" t="s">
         <v>300</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="G32" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="H32" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="90" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>232</v>
       </c>
@@ -15550,90 +15814,90 @@
       <c r="E33" s="4" t="s">
         <v>301</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="G33" s="6" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="35" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H33" s="6" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C35" s="6"/>
-      <c r="F35" s="6"/>
       <c r="G35" s="6"/>
-    </row>
-    <row r="36" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H35" s="6"/>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C36" s="6"/>
-      <c r="F36" s="6"/>
       <c r="G36" s="6"/>
-    </row>
-    <row r="37" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H36" s="6"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C37" s="6"/>
-      <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-    </row>
-    <row r="38" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C38" s="6"/>
-      <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-    </row>
-    <row r="39" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C39" s="6"/>
-      <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-    </row>
-    <row r="40" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C40" s="6"/>
-      <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-    </row>
-    <row r="41" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C41" s="6"/>
-      <c r="F41" s="6"/>
       <c r="G41" s="6"/>
-    </row>
-    <row r="42" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C42" s="6"/>
-      <c r="F42" s="6"/>
       <c r="G42" s="6"/>
-    </row>
-    <row r="43" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C43" s="6"/>
-      <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-    </row>
-    <row r="44" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C44" s="6"/>
-      <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-    </row>
-    <row r="45" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C45" s="6"/>
-      <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-    </row>
-    <row r="46" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C46" s="6"/>
-      <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-    </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C47" s="6"/>
-      <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-    </row>
-    <row r="48" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C48" s="6"/>
-      <c r="F48" s="6"/>
       <c r="G48" s="6"/>
-    </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C49" s="6"/>
-      <c r="F49" s="6"/>
       <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1" xr:uid="{680AF2A0-B839-4572-9E69-3A99B736CEC3}"/>
+  <autoFilter ref="A1:H33" xr:uid="{680AF2A0-B839-4572-9E69-3A99B736CEC3}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>